<commit_message>
Update of attributes and optional parameter formatting on atom-type worksheet
</commit_message>
<xml_diff>
--- a/Atomistic-Class1/WebFF-Class1-DataTemplate.xlsx
+++ b/Atomistic-Class1/WebFF-Class1-DataTemplate.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\NIST_Projects\WebFF\Testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Projects\WebFF-Documentation\Atomistic-Class1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="18195" windowHeight="8190" firstSheet="23" activeTab="29"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="18195" windowHeight="8190" firstSheet="24" activeTab="28"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="20" r:id="rId1"/>
@@ -832,7 +832,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -898,6 +898,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1152,7 +1159,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1225,6 +1231,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
@@ -1585,90 +1592,90 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" style="32" customWidth="1"/>
-    <col min="2" max="2" width="52" style="32" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="32"/>
+    <col min="1" max="1" width="18.5703125" style="31" customWidth="1"/>
+    <col min="2" max="2" width="52" style="31" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="31" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="53" t="s">
+    <row r="1" spans="1:2" s="30" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="52" t="s">
         <v>123</v>
       </c>
-      <c r="B1" s="53"/>
-    </row>
-    <row r="2" spans="1:2" s="31" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="52"/>
+    </row>
+    <row r="2" spans="1:2" s="30" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
       <c r="B2"/>
     </row>
-    <row r="3" spans="1:2" s="31" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
+    <row r="3" spans="1:2" s="30" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
         <v>97</v>
       </c>
-      <c r="B3" s="39"/>
-    </row>
-    <row r="4" spans="1:2" s="31" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="38"/>
+    </row>
+    <row r="4" spans="1:2" s="30" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="14"/>
       <c r="B4" s="18"/>
     </row>
     <row r="5" spans="1:2" ht="22.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="35"/>
+      <c r="B5" s="34"/>
     </row>
     <row r="6" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="38"/>
+      <c r="B6" s="37"/>
     </row>
     <row r="7" spans="1:2" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="B7" s="36"/>
+      <c r="B7" s="35"/>
     </row>
     <row r="8" spans="1:2" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="B8" s="37"/>
+      <c r="B8" s="36"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="B9" s="38"/>
+      <c r="B9" s="37"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="34" t="s">
+      <c r="A10" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="B10" s="38"/>
+      <c r="B10" s="37"/>
     </row>
     <row r="11" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="B11" s="36"/>
+      <c r="B11" s="35"/>
     </row>
     <row r="12" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="29" t="s">
+      <c r="A12" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="B12" s="38"/>
+      <c r="B12" s="37"/>
     </row>
     <row r="13" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="29" t="s">
+      <c r="A13" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="B13" s="38"/>
+      <c r="B13" s="37"/>
     </row>
     <row r="14" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="29" t="s">
+      <c r="A14" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="B14" s="50"/>
+      <c r="B14" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1762,34 +1769,34 @@
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="24" t="s">
+      <c r="D8" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="24" t="s">
+      <c r="E8" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="24" t="s">
+      <c r="F8" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="G8" s="24" t="s">
+      <c r="G8" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="H8" s="25" t="s">
+      <c r="H8" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="I8" s="25" t="s">
+      <c r="I8" s="24" t="s">
         <v>140</v>
       </c>
-      <c r="J8" s="25" t="s">
+      <c r="J8" s="24" t="s">
         <v>141</v>
       </c>
     </row>
@@ -1909,31 +1916,31 @@
     </row>
     <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="24" t="s">
+      <c r="D9" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="E9" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="F9" s="24" t="s">
+      <c r="F9" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="G9" s="25" t="s">
+      <c r="G9" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="H9" s="25" t="s">
+      <c r="H9" s="24" t="s">
         <v>140</v>
       </c>
-      <c r="I9" s="25" t="s">
+      <c r="I9" s="24" t="s">
         <v>141</v>
       </c>
     </row>
@@ -2040,37 +2047,37 @@
     </row>
     <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="24" t="s">
+      <c r="D8" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="24" t="s">
+      <c r="E8" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="F8" s="24" t="s">
+      <c r="F8" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="G8" s="24" t="s">
+      <c r="G8" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="H8" s="24" t="s">
+      <c r="H8" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="I8" s="25" t="s">
+      <c r="I8" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="J8" s="25" t="s">
+      <c r="J8" s="24" t="s">
         <v>140</v>
       </c>
-      <c r="K8" s="25" t="s">
+      <c r="K8" s="24" t="s">
         <v>141</v>
       </c>
     </row>
@@ -2103,7 +2110,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J35" sqref="A9:J35"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2199,13 +2206,13 @@
       <c r="I8" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="J8" s="46" t="s">
+      <c r="J8" s="45" t="s">
         <v>139</v>
       </c>
-      <c r="K8" s="46" t="s">
+      <c r="K8" s="45" t="s">
         <v>140</v>
       </c>
-      <c r="L8" s="46" t="s">
+      <c r="L8" s="45" t="s">
         <v>141</v>
       </c>
     </row>
@@ -2313,71 +2320,71 @@
       </c>
     </row>
     <row r="8" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:22" s="49" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="47" t="s">
+    <row r="9" spans="1:22" s="48" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="47" t="s">
+      <c r="B9" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="47" t="s">
+      <c r="C9" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="47" t="s">
+      <c r="D9" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="47" t="s">
+      <c r="E9" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="47" t="s">
+      <c r="F9" s="46" t="s">
         <v>146</v>
       </c>
-      <c r="G9" s="47" t="s">
+      <c r="G9" s="46" t="s">
         <v>147</v>
       </c>
-      <c r="H9" s="47" t="s">
+      <c r="H9" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="I9" s="47" t="s">
+      <c r="I9" s="46" t="s">
         <v>148</v>
       </c>
-      <c r="J9" s="47" t="s">
+      <c r="J9" s="46" t="s">
         <v>149</v>
       </c>
-      <c r="K9" s="47" t="s">
+      <c r="K9" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="L9" s="47" t="s">
+      <c r="L9" s="46" t="s">
         <v>150</v>
       </c>
-      <c r="M9" s="47" t="s">
+      <c r="M9" s="46" t="s">
         <v>151</v>
       </c>
-      <c r="N9" s="47" t="s">
+      <c r="N9" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="O9" s="47" t="s">
+      <c r="O9" s="46" t="s">
         <v>152</v>
       </c>
-      <c r="P9" s="47" t="s">
+      <c r="P9" s="46" t="s">
         <v>153</v>
       </c>
-      <c r="Q9" s="47" t="s">
+      <c r="Q9" s="46" t="s">
         <v>107</v>
       </c>
-      <c r="R9" s="47" t="s">
+      <c r="R9" s="46" t="s">
         <v>154</v>
       </c>
-      <c r="S9" s="47" t="s">
+      <c r="S9" s="46" t="s">
         <v>155</v>
       </c>
-      <c r="T9" s="48" t="s">
+      <c r="T9" s="47" t="s">
         <v>139</v>
       </c>
-      <c r="U9" s="48" t="s">
+      <c r="U9" s="47" t="s">
         <v>140</v>
       </c>
-      <c r="V9" s="48" t="s">
+      <c r="V9" s="47" t="s">
         <v>141</v>
       </c>
     </row>
@@ -2517,76 +2524,76 @@
       <c r="G7"/>
     </row>
     <row r="8" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="24" t="s">
+      <c r="D8" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="24" t="s">
+      <c r="E8" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="F8" s="24" t="s">
+      <c r="F8" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="G8" s="24" t="s">
+      <c r="G8" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="H8" s="25" t="s">
+      <c r="H8" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="I8" s="25" t="s">
+      <c r="I8" s="24" t="s">
         <v>140</v>
       </c>
-      <c r="J8" s="25" t="s">
+      <c r="J8" s="24" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="51"/>
-      <c r="B9" s="51"/>
-      <c r="C9" s="51"/>
-      <c r="D9" s="51"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="51"/>
+      <c r="A9" s="50"/>
+      <c r="B9" s="50"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="50"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="50"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="51"/>
-      <c r="B10" s="51"/>
-      <c r="C10" s="51"/>
-      <c r="D10" s="51"/>
-      <c r="F10" s="51"/>
-      <c r="G10" s="51"/>
+      <c r="A10" s="50"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="50"/>
+      <c r="F10" s="50"/>
+      <c r="G10" s="50"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="51"/>
-      <c r="B11" s="51"/>
-      <c r="C11" s="51"/>
-      <c r="D11" s="51"/>
-      <c r="F11" s="51"/>
-      <c r="G11" s="51"/>
+      <c r="A11" s="50"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="50"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="50"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="51"/>
-      <c r="B12" s="51"/>
-      <c r="C12" s="51"/>
-      <c r="D12" s="51"/>
-      <c r="F12" s="51"/>
-      <c r="G12" s="51"/>
+      <c r="A12" s="50"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="50"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="50"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="51"/>
-      <c r="B13" s="51"/>
-      <c r="C13" s="51"/>
-      <c r="D13" s="51"/>
-      <c r="F13" s="51"/>
-      <c r="G13" s="51"/>
+      <c r="A13" s="50"/>
+      <c r="B13" s="50"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="50"/>
+      <c r="F13" s="50"/>
+      <c r="G13" s="50"/>
     </row>
   </sheetData>
   <dataValidations count="6">
@@ -2733,63 +2740,63 @@
       <c r="F8"/>
     </row>
     <row r="9" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="24" t="s">
+      <c r="D9" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="E9" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="F9" s="24" t="s">
+      <c r="F9" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="G9" s="25" t="s">
+      <c r="G9" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="H9" s="25" t="s">
+      <c r="H9" s="24" t="s">
         <v>140</v>
       </c>
-      <c r="I9" s="25" t="s">
+      <c r="I9" s="24" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="51"/>
-      <c r="B10" s="51"/>
-      <c r="C10" s="51"/>
-      <c r="D10" s="51"/>
+      <c r="A10" s="50"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="50"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="51"/>
-      <c r="B11" s="51"/>
-      <c r="C11" s="51"/>
-      <c r="D11" s="51"/>
+      <c r="A11" s="50"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="50"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="51"/>
-      <c r="B12" s="51"/>
-      <c r="C12" s="51"/>
-      <c r="D12" s="51"/>
+      <c r="A12" s="50"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="50"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="51"/>
-      <c r="B13" s="51"/>
-      <c r="C13" s="51"/>
-      <c r="D13" s="51"/>
+      <c r="A13" s="50"/>
+      <c r="B13" s="50"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="50"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="51"/>
-      <c r="B14" s="51"/>
-      <c r="C14" s="51"/>
-      <c r="D14" s="51"/>
+      <c r="A14" s="50"/>
+      <c r="B14" s="50"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="50"/>
     </row>
   </sheetData>
   <dataValidations count="5">
@@ -2903,31 +2910,31 @@
     </row>
     <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="24" t="s">
+      <c r="D9" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="E9" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="F9" s="24" t="s">
+      <c r="F9" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="G9" s="25" t="s">
+      <c r="G9" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="H9" s="25" t="s">
+      <c r="H9" s="24" t="s">
         <v>140</v>
       </c>
-      <c r="I9" s="25" t="s">
+      <c r="I9" s="24" t="s">
         <v>141</v>
       </c>
     </row>
@@ -3032,37 +3039,37 @@
     </row>
     <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="24" t="s">
+      <c r="D8" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="24" t="s">
+      <c r="E8" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="F8" s="24" t="s">
+      <c r="F8" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="G8" s="24" t="s">
+      <c r="G8" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="H8" s="24" t="s">
+      <c r="H8" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="I8" s="25" t="s">
+      <c r="I8" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="J8" s="25" t="s">
+      <c r="J8" s="24" t="s">
         <v>140</v>
       </c>
-      <c r="K8" s="25" t="s">
+      <c r="K8" s="24" t="s">
         <v>141</v>
       </c>
     </row>
@@ -3176,31 +3183,31 @@
     </row>
     <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="24" t="s">
+      <c r="D9" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="E9" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="F9" s="24" t="s">
+      <c r="F9" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="G9" s="25" t="s">
+      <c r="G9" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="H9" s="25" t="s">
+      <c r="H9" s="24" t="s">
         <v>140</v>
       </c>
-      <c r="I9" s="25" t="s">
+      <c r="I9" s="24" t="s">
         <v>141</v>
       </c>
     </row>
@@ -3243,20 +3250,20 @@
   <cols>
     <col min="1" max="1" width="25.140625" customWidth="1"/>
     <col min="2" max="2" width="43.140625" customWidth="1"/>
-    <col min="3" max="16384" width="9" style="30"/>
+    <col min="3" max="16384" width="9" style="29"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="54"/>
+      <c r="B1" s="53"/>
     </row>
     <row r="2" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
     </row>
     <row r="3" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="22" t="s">
         <v>97</v>
       </c>
       <c r="B3" s="12"/>
@@ -3266,10 +3273,10 @@
       <c r="B4" s="18"/>
     </row>
     <row r="5" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="24" t="s">
         <v>98</v>
       </c>
     </row>
@@ -3451,34 +3458,34 @@
     </row>
     <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="24" t="s">
+      <c r="D9" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="E9" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="F9" s="24" t="s">
+      <c r="F9" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="G9" s="24" t="s">
+      <c r="G9" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="H9" s="25" t="s">
+      <c r="H9" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="I9" s="25" t="s">
+      <c r="I9" s="24" t="s">
         <v>140</v>
       </c>
-      <c r="J9" s="25" t="s">
+      <c r="J9" s="24" t="s">
         <v>141</v>
       </c>
     </row>
@@ -3589,22 +3596,22 @@
     </row>
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="D9" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="E9" s="25" t="s">
+      <c r="E9" s="24" t="s">
         <v>140</v>
       </c>
-      <c r="F9" s="25" t="s">
+      <c r="F9" s="24" t="s">
         <v>141</v>
       </c>
     </row>
@@ -3716,22 +3723,22 @@
     </row>
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="D9" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="E9" s="25" t="s">
+      <c r="E9" s="24" t="s">
         <v>140</v>
       </c>
-      <c r="F9" s="25" t="s">
+      <c r="F9" s="24" t="s">
         <v>141</v>
       </c>
     </row>
@@ -3779,14 +3786,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="52" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -3845,22 +3852,22 @@
     </row>
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="23" t="s">
         <v>130</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="23" t="s">
         <v>158</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="D9" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="E9" s="25" t="s">
+      <c r="E9" s="24" t="s">
         <v>140</v>
       </c>
-      <c r="F9" s="25" t="s">
+      <c r="F9" s="24" t="s">
         <v>141</v>
       </c>
     </row>
@@ -3899,7 +3906,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H34" sqref="A10:H34"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3975,22 +3982,22 @@
     </row>
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="D9" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="E9" s="25" t="s">
+      <c r="E9" s="24" t="s">
         <v>140</v>
       </c>
-      <c r="F9" s="25" t="s">
+      <c r="F9" s="24" t="s">
         <v>141</v>
       </c>
     </row>
@@ -4026,7 +4033,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G42" sqref="G42"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4039,15 +4046,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="52" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -4106,25 +4113,25 @@
     </row>
     <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="D9" s="24" t="s">
+      <c r="D9" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="E9" s="25" t="s">
+      <c r="E9" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="F9" s="25" t="s">
+      <c r="F9" s="24" t="s">
         <v>140</v>
       </c>
-      <c r="G9" s="25" t="s">
+      <c r="G9" s="24" t="s">
         <v>141</v>
       </c>
     </row>
@@ -4175,60 +4182,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="52" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="54" t="s">
         <v>96</v>
       </c>
-      <c r="C3" s="56"/>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="56"/>
-      <c r="G3" s="56"/>
-      <c r="H3" s="56"/>
-      <c r="I3" s="57"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="56"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="D5" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="E5" s="24" t="s">
+      <c r="E5" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="F5" s="24" t="s">
+      <c r="F5" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="G5" s="25" t="s">
+      <c r="G5" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="H5" s="25" t="s">
+      <c r="H5" s="24" t="s">
         <v>140</v>
       </c>
-      <c r="I5" s="25" t="s">
+      <c r="I5" s="24" t="s">
         <v>141</v>
       </c>
     </row>
@@ -4269,80 +4276,80 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="52" t="s">
         <v>131</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="52"/>
+      <c r="L1" s="52"/>
+      <c r="M1" s="52"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="54" t="s">
         <v>96</v>
       </c>
-      <c r="C3" s="56"/>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="56"/>
-      <c r="G3" s="56"/>
-      <c r="H3" s="56"/>
-      <c r="I3" s="56"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="56"/>
-      <c r="L3" s="56"/>
-      <c r="M3" s="57"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="55"/>
+      <c r="L3" s="55"/>
+      <c r="M3" s="56"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="23" t="s">
         <v>132</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="D5" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="E5" s="24" t="s">
+      <c r="E5" s="23" t="s">
         <v>133</v>
       </c>
-      <c r="F5" s="24" t="s">
+      <c r="F5" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="G5" s="24" t="s">
+      <c r="G5" s="23" t="s">
         <v>135</v>
       </c>
-      <c r="H5" s="24" t="s">
+      <c r="H5" s="23" t="s">
         <v>136</v>
       </c>
-      <c r="I5" s="24" t="s">
+      <c r="I5" s="23" t="s">
         <v>137</v>
       </c>
-      <c r="J5" s="24" t="s">
+      <c r="J5" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="K5" s="25" t="s">
+      <c r="K5" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="L5" s="25" t="s">
+      <c r="L5" s="24" t="s">
         <v>140</v>
       </c>
-      <c r="M5" s="25" t="s">
+      <c r="M5" s="24" t="s">
         <v>141</v>
       </c>
     </row>
@@ -4377,15 +4384,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="52" t="s">
         <v>99</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
       <c r="H1" s="10"/>
       <c r="I1" s="10"/>
     </row>
@@ -4393,34 +4400,34 @@
       <c r="A3" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="B3" s="42"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="44"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="43"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="D5" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="E5" s="25" t="s">
+      <c r="E5" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="F5" s="25" t="s">
+      <c r="F5" s="24" t="s">
         <v>140</v>
       </c>
-      <c r="G5" s="25" t="s">
+      <c r="G5" s="24" t="s">
         <v>141</v>
       </c>
     </row>
@@ -4439,9 +4446,9 @@
   </sheetPr>
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G25" sqref="A7:G25"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4452,19 +4459,19 @@
     <col min="4" max="4" width="35.28515625" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" customWidth="1"/>
     <col min="7" max="7" width="12.42578125" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="45"/>
+    <col min="8" max="16384" width="9.140625" style="44"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -4490,72 +4497,72 @@
     </row>
     <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="58" t="s">
         <v>111</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="58" t="s">
         <v>110</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="E6" s="25" t="s">
+      <c r="E6" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="F6" s="25" t="s">
+      <c r="F6" s="24" t="s">
         <v>159</v>
       </c>
-      <c r="G6" s="25" t="s">
+      <c r="G6" s="24" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="52"/>
-      <c r="B7" s="52"/>
-      <c r="C7" s="52"/>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
-      <c r="F7" s="52"/>
-      <c r="G7" s="52"/>
+      <c r="A7" s="51"/>
+      <c r="B7" s="51"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
+      <c r="F7" s="51"/>
+      <c r="G7" s="51"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="52"/>
-      <c r="B8" s="52"/>
-      <c r="C8" s="52"/>
-      <c r="D8" s="52"/>
-      <c r="E8" s="52"/>
-      <c r="F8" s="52"/>
-      <c r="G8" s="52"/>
+      <c r="A8" s="51"/>
+      <c r="B8" s="51"/>
+      <c r="C8" s="51"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="51"/>
+      <c r="F8" s="51"/>
+      <c r="G8" s="51"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="52"/>
-      <c r="B9" s="52"/>
-      <c r="C9" s="52"/>
-      <c r="D9" s="52"/>
-      <c r="E9" s="52"/>
-      <c r="F9" s="52"/>
-      <c r="G9" s="52"/>
+      <c r="A9" s="51"/>
+      <c r="B9" s="51"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="51"/>
+      <c r="G9" s="51"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="52"/>
-      <c r="B10" s="52"/>
-      <c r="C10" s="52"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="52"/>
-      <c r="F10" s="52"/>
-      <c r="G10" s="52"/>
+      <c r="A10" s="51"/>
+      <c r="B10" s="51"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="51"/>
+      <c r="G10" s="51"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="52"/>
-      <c r="B11" s="52"/>
-      <c r="C11" s="52"/>
-      <c r="D11" s="52"/>
-      <c r="E11" s="52"/>
-      <c r="F11" s="52"/>
-      <c r="G11" s="52"/>
+      <c r="A11" s="51"/>
+      <c r="B11" s="51"/>
+      <c r="C11" s="51"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="51"/>
+      <c r="G11" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4998,9 +5005,9 @@
   </sheetPr>
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I35" sqref="I35"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5029,42 +5036,42 @@
       <c r="A3" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="B3" s="58"/>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="58"/>
-      <c r="I3" s="58"/>
+      <c r="B3" s="57"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="24" t="s">
         <v>121</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="24" t="s">
         <v>120</v>
       </c>
-      <c r="E5" s="25" t="s">
+      <c r="E5" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="F5" s="25" t="s">
+      <c r="F5" s="24" t="s">
         <v>118</v>
       </c>
-      <c r="G5" s="25" t="s">
+      <c r="G5" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="H5" s="25" t="s">
+      <c r="H5" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="I5" s="25" t="s">
+      <c r="I5" s="24" t="s">
         <v>115</v>
       </c>
     </row>
@@ -5086,7 +5093,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F20" sqref="A9:F20"/>
+      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5098,19 +5105,19 @@
     <col min="5" max="5" width="36.140625" customWidth="1"/>
     <col min="6" max="6" width="9.7109375" customWidth="1"/>
     <col min="7" max="7" width="10.42578125" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="41"/>
+    <col min="8" max="16384" width="9.140625" style="40"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
@@ -5191,25 +5198,25 @@
       <c r="G7" s="21"/>
     </row>
     <row r="8" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="24" t="s">
+      <c r="D8" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="25" t="s">
+      <c r="E8" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="F8" s="25" t="s">
+      <c r="F8" s="24" t="s">
         <v>140</v>
       </c>
-      <c r="G8" s="25" t="s">
+      <c r="G8" s="24" t="s">
         <v>141</v>
       </c>
     </row>
@@ -5244,7 +5251,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F26" sqref="A10:F26"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5257,20 +5264,20 @@
     <col min="6" max="6" width="34.42578125" customWidth="1"/>
     <col min="7" max="7" width="9"/>
     <col min="8" max="8" width="10.140625" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="40"/>
+    <col min="9" max="16384" width="9.140625" style="39"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -5336,28 +5343,28 @@
       <c r="B8" s="3"/>
     </row>
     <row r="9" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="23" t="s">
         <v>129</v>
       </c>
-      <c r="D9" s="24" t="s">
+      <c r="D9" s="23" t="s">
         <v>130</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="E9" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="25" t="s">
+      <c r="F9" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="G9" s="25" t="s">
+      <c r="G9" s="24" t="s">
         <v>140</v>
       </c>
-      <c r="H9" s="25" t="s">
+      <c r="H9" s="24" t="s">
         <v>141</v>
       </c>
     </row>
@@ -5395,7 +5402,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G30" sqref="A9:G30"/>
+      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5409,21 +5416,21 @@
     <col min="7" max="7" width="31.42578125" customWidth="1"/>
     <col min="8" max="8" width="11.140625" customWidth="1"/>
     <col min="9" max="9" width="11.28515625" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="26"/>
+    <col min="10" max="16384" width="9.140625" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -5471,31 +5478,31 @@
     </row>
     <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="24" t="s">
+      <c r="D8" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="24" t="s">
+      <c r="E8" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="25" t="s">
+      <c r="F8" s="24" t="s">
         <v>142</v>
       </c>
-      <c r="G8" s="25" t="s">
+      <c r="G8" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="H8" s="25" t="s">
+      <c r="H8" s="24" t="s">
         <v>140</v>
       </c>
-      <c r="I8" s="25" t="s">
+      <c r="I8" s="24" t="s">
         <v>141</v>
       </c>
     </row>
@@ -5545,21 +5552,21 @@
     <col min="7" max="7" width="34.42578125" customWidth="1"/>
     <col min="8" max="8" width="10.7109375" customWidth="1"/>
     <col min="9" max="9" width="15.140625" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="28"/>
+    <col min="10" max="16384" width="9.140625" style="27"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -5611,31 +5618,31 @@
     </row>
     <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="24" t="s">
+      <c r="D8" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="24" t="s">
+      <c r="E8" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="25" t="s">
+      <c r="F8" s="24" t="s">
         <v>142</v>
       </c>
-      <c r="G8" s="25" t="s">
+      <c r="G8" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="H8" s="25" t="s">
+      <c r="H8" s="24" t="s">
         <v>140</v>
       </c>
-      <c r="I8" s="25" t="s">
+      <c r="I8" s="24" t="s">
         <v>141</v>
       </c>
     </row>
@@ -5687,19 +5694,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="52"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -5777,37 +5784,37 @@
       <c r="B9" s="3"/>
     </row>
     <row r="10" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="D10" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="24" t="s">
+      <c r="E10" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="24" t="s">
+      <c r="F10" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="G10" s="24" t="s">
+      <c r="G10" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="H10" s="25" t="s">
+      <c r="H10" s="24" t="s">
         <v>142</v>
       </c>
-      <c r="I10" s="25" t="s">
+      <c r="I10" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="J10" s="25" t="s">
+      <c r="J10" s="24" t="s">
         <v>140</v>
       </c>
-      <c r="K10" s="25" t="s">
+      <c r="K10" s="24" t="s">
         <v>141</v>
       </c>
     </row>
@@ -5931,34 +5938,34 @@
     </row>
     <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="24" t="s">
+      <c r="D9" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="E9" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="F9" s="24" t="s">
+      <c r="F9" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="G9" s="24" t="s">
+      <c r="G9" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="H9" s="25" t="s">
+      <c r="H9" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="I9" s="25" t="s">
+      <c r="I9" s="24" t="s">
         <v>140</v>
       </c>
-      <c r="J9" s="25" t="s">
+      <c r="J9" s="24" t="s">
         <v>141</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updates to AtomTypes as of 4/11/2018
</commit_message>
<xml_diff>
--- a/Atomistic-Class1/WebFF-Class1-DataTemplate.xlsx
+++ b/Atomistic-Class1/WebFF-Class1-DataTemplate.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Projects\WebFF-Documentation\Atomistic-Class1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\Projects\WebFF-Documentation\Atomistic-Class1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="18195" windowHeight="8190" firstSheet="24" activeTab="28"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="18195" windowHeight="8190" firstSheet="28" activeTab="32"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="20" r:id="rId1"/>
@@ -40,8 +40,11 @@
     <sheet name="EquivalenceTable" sheetId="27" r:id="rId26"/>
     <sheet name="AutoEquivalenceTable" sheetId="33" r:id="rId27"/>
     <sheet name="BondIncrements" sheetId="28" r:id="rId28"/>
-    <sheet name="AtomTypes" sheetId="30" r:id="rId29"/>
-    <sheet name="Atom-Attributes" sheetId="31" r:id="rId30"/>
+    <sheet name="AtomType-ATDL" sheetId="37" r:id="rId29"/>
+    <sheet name="AtomType-DFF" sheetId="39" r:id="rId30"/>
+    <sheet name="AtomType-Generic" sheetId="38" r:id="rId31"/>
+    <sheet name="Atom-Attributes-DFF" sheetId="41" r:id="rId32"/>
+    <sheet name="Atom-Attributes-Generic" sheetId="31" r:id="rId33"/>
   </sheets>
   <definedNames>
     <definedName name="KeywordListTab_1" localSheetId="2">KeywordsList!$A$2:$A$74</definedName>
@@ -64,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="261">
   <si>
     <t>Harmonic</t>
   </si>
@@ -396,9 +399,6 @@
     <t>Element</t>
   </si>
   <si>
-    <t>BondPattern-2</t>
-  </si>
-  <si>
     <t>BondPattern</t>
   </si>
   <si>
@@ -549,9 +549,6 @@
     <t>AtomicMass</t>
   </si>
   <si>
-    <t>PatternNomenclatureStyle</t>
-  </si>
-  <si>
     <t>1/nm</t>
   </si>
   <si>
@@ -826,6 +823,33 @@
   </si>
   <si>
     <t>Lennard-Jones (9-6) [Class 2 Form]</t>
+  </si>
+  <si>
+    <t>Atom</t>
+  </si>
+  <si>
+    <t>BondedAtoms</t>
+  </si>
+  <si>
+    <t>Generic</t>
+  </si>
+  <si>
+    <t>Nomenclature</t>
+  </si>
+  <si>
+    <t>Atom-Types-Generic</t>
+  </si>
+  <si>
+    <t>DFF</t>
+  </si>
+  <si>
+    <t>Substructure</t>
+  </si>
+  <si>
+    <t>Ringsize</t>
+  </si>
+  <si>
+    <t>Coordination</t>
   </si>
 </sst>
 </file>
@@ -1213,6 +1237,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1231,7 +1256,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
@@ -1598,10 +1622,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="30" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="52" t="s">
-        <v>123</v>
-      </c>
-      <c r="B1" s="52"/>
+      <c r="A1" s="53" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" s="53"/>
     </row>
     <row r="2" spans="1:2" s="30" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
@@ -1721,7 +1745,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -1733,7 +1757,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>35</v>
@@ -1745,10 +1769,10 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
@@ -1760,7 +1784,7 @@
         <v>33</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5" t="s">
@@ -1791,13 +1815,13 @@
         <v>30</v>
       </c>
       <c r="H8" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="I8" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="I8" s="24" t="s">
+      <c r="J8" s="24" t="s">
         <v>140</v>
-      </c>
-      <c r="J8" s="24" t="s">
-        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -1856,7 +1880,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>37</v>
@@ -1868,7 +1892,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>38</v>
@@ -1880,10 +1904,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
@@ -1895,7 +1919,7 @@
         <v>33</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5" t="s">
@@ -1935,13 +1959,13 @@
         <v>31</v>
       </c>
       <c r="G9" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="H9" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="H9" s="24" t="s">
+      <c r="I9" s="24" t="s">
         <v>140</v>
-      </c>
-      <c r="I9" s="24" t="s">
-        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -1999,7 +2023,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>44</v>
@@ -2011,7 +2035,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>39</v>
@@ -2023,10 +2047,10 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C5" s="5"/>
       <c r="F5" s="5" t="s">
@@ -2035,10 +2059,10 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C6" s="5"/>
       <c r="F6" s="5" t="s">
@@ -2072,13 +2096,13 @@
         <v>43</v>
       </c>
       <c r="I8" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="J8" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="J8" s="24" t="s">
+      <c r="K8" s="24" t="s">
         <v>140</v>
-      </c>
-      <c r="K8" s="24" t="s">
-        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -2132,7 +2156,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>108</v>
@@ -2144,7 +2168,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>106</v>
@@ -2156,10 +2180,10 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C5" s="5"/>
       <c r="G5" s="5" t="s">
@@ -2168,10 +2192,10 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C6" s="5"/>
       <c r="G6" s="5" t="s">
@@ -2207,13 +2231,13 @@
         <v>107</v>
       </c>
       <c r="J8" s="45" t="s">
+        <v>138</v>
+      </c>
+      <c r="K8" s="45" t="s">
         <v>139</v>
       </c>
-      <c r="K8" s="45" t="s">
+      <c r="L8" s="45" t="s">
         <v>140</v>
-      </c>
-      <c r="L8" s="45" t="s">
-        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -2261,7 +2285,7 @@
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>58</v>
@@ -2273,10 +2297,10 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C4" s="5"/>
       <c r="I4" s="5" t="s">
@@ -2285,10 +2309,10 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C5" s="5"/>
       <c r="I5" s="5" t="s">
@@ -2297,10 +2321,10 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C6" s="5"/>
       <c r="I6" s="5" t="s">
@@ -2309,7 +2333,7 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>10</v>
@@ -2337,55 +2361,55 @@
         <v>40</v>
       </c>
       <c r="F9" s="46" t="s">
+        <v>145</v>
+      </c>
+      <c r="G9" s="46" t="s">
         <v>146</v>
-      </c>
-      <c r="G9" s="46" t="s">
-        <v>147</v>
       </c>
       <c r="H9" s="46" t="s">
         <v>41</v>
       </c>
       <c r="I9" s="46" t="s">
+        <v>147</v>
+      </c>
+      <c r="J9" s="46" t="s">
         <v>148</v>
-      </c>
-      <c r="J9" s="46" t="s">
-        <v>149</v>
       </c>
       <c r="K9" s="46" t="s">
         <v>42</v>
       </c>
       <c r="L9" s="46" t="s">
+        <v>149</v>
+      </c>
+      <c r="M9" s="46" t="s">
         <v>150</v>
-      </c>
-      <c r="M9" s="46" t="s">
-        <v>151</v>
       </c>
       <c r="N9" s="46" t="s">
         <v>43</v>
       </c>
       <c r="O9" s="46" t="s">
+        <v>151</v>
+      </c>
+      <c r="P9" s="46" t="s">
         <v>152</v>
-      </c>
-      <c r="P9" s="46" t="s">
-        <v>153</v>
       </c>
       <c r="Q9" s="46" t="s">
         <v>107</v>
       </c>
       <c r="R9" s="46" t="s">
+        <v>153</v>
+      </c>
+      <c r="S9" s="46" t="s">
         <v>154</v>
       </c>
-      <c r="S9" s="46" t="s">
-        <v>155</v>
-      </c>
       <c r="T9" s="47" t="s">
+        <v>138</v>
+      </c>
+      <c r="U9" s="47" t="s">
         <v>139</v>
       </c>
-      <c r="U9" s="47" t="s">
+      <c r="V9" s="47" t="s">
         <v>140</v>
-      </c>
-      <c r="V9" s="47" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -2456,7 +2480,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>49</v>
@@ -2471,7 +2495,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>50</v>
@@ -2486,10 +2510,10 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
@@ -2504,7 +2528,7 @@
         <v>53</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5" t="s">
@@ -2546,13 +2570,13 @@
         <v>30</v>
       </c>
       <c r="H8" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="I8" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="I8" s="24" t="s">
+      <c r="J8" s="24" t="s">
         <v>140</v>
-      </c>
-      <c r="J8" s="24" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -2663,7 +2687,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>16</v>
@@ -2677,7 +2701,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>52</v>
@@ -2691,10 +2715,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
@@ -2708,7 +2732,7 @@
         <v>53</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5" t="s">
@@ -2759,13 +2783,13 @@
         <v>55</v>
       </c>
       <c r="G9" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="H9" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="H9" s="24" t="s">
+      <c r="I9" s="24" t="s">
         <v>140</v>
-      </c>
-      <c r="I9" s="24" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -2850,7 +2874,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -2862,7 +2886,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>56</v>
@@ -2874,10 +2898,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
@@ -2889,7 +2913,7 @@
         <v>53</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5" t="s">
@@ -2929,13 +2953,13 @@
         <v>55</v>
       </c>
       <c r="G9" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="H9" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="H9" s="24" t="s">
+      <c r="I9" s="24" t="s">
         <v>140</v>
-      </c>
-      <c r="I9" s="24" t="s">
-        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -2991,7 +3015,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>58</v>
@@ -3003,7 +3027,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>62</v>
@@ -3015,10 +3039,10 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C5" s="5"/>
       <c r="F5" s="5" t="s">
@@ -3030,7 +3054,7 @@
         <v>53</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C6" s="5"/>
       <c r="F6" s="5" t="s">
@@ -3064,13 +3088,13 @@
         <v>61</v>
       </c>
       <c r="I8" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="J8" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="J8" s="24" t="s">
+      <c r="K8" s="24" t="s">
         <v>140</v>
-      </c>
-      <c r="K8" s="24" t="s">
-        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -3123,7 +3147,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>63</v>
@@ -3135,7 +3159,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>64</v>
@@ -3147,10 +3171,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C5" s="5"/>
       <c r="G5" s="5" t="s">
@@ -3162,7 +3186,7 @@
         <v>53</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C6" s="5"/>
       <c r="G6" s="5" t="s">
@@ -3202,13 +3226,13 @@
         <v>65</v>
       </c>
       <c r="G9" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="H9" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="H9" s="24" t="s">
+      <c r="I9" s="24" t="s">
         <v>140</v>
-      </c>
-      <c r="I9" s="24" t="s">
-        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -3254,10 +3278,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="54" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="53"/>
+      <c r="B1" s="54"/>
     </row>
     <row r="2" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
@@ -3398,7 +3422,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>18</v>
@@ -3410,7 +3434,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>105</v>
@@ -3422,10 +3446,10 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
@@ -3437,7 +3461,7 @@
         <v>33</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5" t="s">
@@ -3480,13 +3504,13 @@
         <v>31</v>
       </c>
       <c r="H9" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="I9" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="I9" s="24" t="s">
+      <c r="J9" s="24" t="s">
         <v>140</v>
-      </c>
-      <c r="J9" s="24" t="s">
-        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -3541,7 +3565,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>75</v>
@@ -3552,7 +3576,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>76</v>
@@ -3566,7 +3590,7 @@
         <v>82</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>24</v>
@@ -3577,7 +3601,7 @@
         <v>83</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>24</v>
@@ -3585,10 +3609,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>24</v>
@@ -3606,13 +3630,13 @@
         <v>79</v>
       </c>
       <c r="D9" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="E9" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="F9" s="24" t="s">
         <v>140</v>
-      </c>
-      <c r="F9" s="24" t="s">
-        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -3668,7 +3692,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>85</v>
@@ -3679,7 +3703,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>80</v>
@@ -3693,7 +3717,7 @@
         <v>82</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>24</v>
@@ -3704,7 +3728,7 @@
         <v>84</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>24</v>
@@ -3712,10 +3736,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>24</v>
@@ -3733,13 +3757,13 @@
         <v>81</v>
       </c>
       <c r="D9" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="E9" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="F9" s="24" t="s">
         <v>140</v>
-      </c>
-      <c r="F9" s="24" t="s">
-        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -3786,21 +3810,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="53" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>12</v>
@@ -3808,7 +3832,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>87</v>
@@ -3822,7 +3846,7 @@
         <v>86</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>24</v>
@@ -3833,7 +3857,7 @@
         <v>88</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>24</v>
@@ -3841,10 +3865,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>24</v>
@@ -3856,19 +3880,19 @@
         <v>77</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D9" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="E9" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="F9" s="24" t="s">
         <v>140</v>
-      </c>
-      <c r="F9" s="24" t="s">
-        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -3927,10 +3951,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>12</v>
@@ -3938,7 +3962,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>89</v>
@@ -3952,7 +3976,7 @@
         <v>82</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>24</v>
@@ -3963,7 +3987,7 @@
         <v>83</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>24</v>
@@ -3971,10 +3995,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>24</v>
@@ -3992,13 +4016,13 @@
         <v>79</v>
       </c>
       <c r="D9" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="E9" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="F9" s="24" t="s">
         <v>140</v>
-      </c>
-      <c r="F9" s="24" t="s">
-        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -4046,19 +4070,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="53" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>75</v>
@@ -4069,7 +4093,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>76</v>
@@ -4083,7 +4107,7 @@
         <v>82</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>24</v>
@@ -4094,7 +4118,7 @@
         <v>83</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>24</v>
@@ -4102,10 +4126,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>24</v>
@@ -4126,13 +4150,13 @@
         <v>79</v>
       </c>
       <c r="E9" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="F9" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="F9" s="24" t="s">
+      <c r="G9" s="24" t="s">
         <v>140</v>
-      </c>
-      <c r="G9" s="24" t="s">
-        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -4182,32 +4206,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="53" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="55" t="s">
         <v>96</v>
       </c>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="55"/>
-      <c r="I3" s="56"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="56"/>
+      <c r="I3" s="57"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4230,13 +4254,13 @@
         <v>94</v>
       </c>
       <c r="G5" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="H5" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="H5" s="24" t="s">
+      <c r="I5" s="24" t="s">
         <v>140</v>
-      </c>
-      <c r="I5" s="24" t="s">
-        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -4276,40 +4300,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="52" t="s">
-        <v>131</v>
-      </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="52"/>
-      <c r="M1" s="52"/>
+      <c r="A1" s="53" t="s">
+        <v>130</v>
+      </c>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="53"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="55" t="s">
         <v>96</v>
       </c>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="55"/>
-      <c r="L3" s="55"/>
-      <c r="M3" s="56"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="56"/>
+      <c r="I3" s="56"/>
+      <c r="J3" s="56"/>
+      <c r="K3" s="56"/>
+      <c r="L3" s="56"/>
+      <c r="M3" s="57"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4320,37 +4344,37 @@
         <v>90</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D5" s="23" t="s">
         <v>91</v>
       </c>
       <c r="E5" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="F5" s="23" t="s">
         <v>133</v>
       </c>
-      <c r="F5" s="23" t="s">
+      <c r="G5" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="G5" s="23" t="s">
+      <c r="H5" s="23" t="s">
         <v>135</v>
       </c>
-      <c r="H5" s="23" t="s">
+      <c r="I5" s="23" t="s">
         <v>136</v>
       </c>
-      <c r="I5" s="23" t="s">
+      <c r="J5" s="23" t="s">
         <v>137</v>
       </c>
-      <c r="J5" s="23" t="s">
+      <c r="K5" s="24" t="s">
         <v>138</v>
       </c>
-      <c r="K5" s="24" t="s">
+      <c r="L5" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="L5" s="24" t="s">
+      <c r="M5" s="24" t="s">
         <v>140</v>
-      </c>
-      <c r="M5" s="24" t="s">
-        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -4384,15 +4408,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="53" t="s">
         <v>99</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
       <c r="H1" s="10"/>
       <c r="I1" s="10"/>
     </row>
@@ -4422,13 +4446,13 @@
         <v>102</v>
       </c>
       <c r="E5" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="F5" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="F5" s="24" t="s">
+      <c r="G5" s="24" t="s">
         <v>140</v>
-      </c>
-      <c r="G5" s="24" t="s">
-        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -4444,82 +4468,85 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.7109375" customWidth="1"/>
     <col min="2" max="2" width="37.42578125" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="35.28515625" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="44"/>
+    <col min="3" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="35.28515625" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="44"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="52" t="s">
-        <v>114</v>
-      </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="53" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>161</v>
+        <v>255</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D3" s="5"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>139</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="B4" s="3"/>
       <c r="C4" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+      <c r="D4" s="5"/>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="23" t="s">
-        <v>112</v>
-      </c>
-      <c r="B6" s="58" t="s">
         <v>111</v>
       </c>
-      <c r="C6" s="58" t="s">
-        <v>110</v>
-      </c>
-      <c r="D6" s="24" t="s">
+      <c r="B6" s="52" t="s">
+        <v>252</v>
+      </c>
+      <c r="C6" s="52" t="s">
+        <v>253</v>
+      </c>
+      <c r="D6" s="52" t="s">
+        <v>117</v>
+      </c>
+      <c r="E6" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="E6" s="24" t="s">
+      <c r="F6" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="F6" s="24" t="s">
+      <c r="G6" s="24" t="s">
+        <v>158</v>
+      </c>
+      <c r="H6" s="24" t="s">
         <v>159</v>
       </c>
-      <c r="G6" s="24" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="51"/>
       <c r="B7" s="51"/>
       <c r="C7" s="51"/>
@@ -4527,8 +4554,9 @@
       <c r="E7" s="51"/>
       <c r="F7" s="51"/>
       <c r="G7" s="51"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" s="51"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="51"/>
       <c r="B8" s="51"/>
       <c r="C8" s="51"/>
@@ -4536,8 +4564,9 @@
       <c r="E8" s="51"/>
       <c r="F8" s="51"/>
       <c r="G8" s="51"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" s="51"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="51"/>
       <c r="B9" s="51"/>
       <c r="C9" s="51"/>
@@ -4545,8 +4574,9 @@
       <c r="E9" s="51"/>
       <c r="F9" s="51"/>
       <c r="G9" s="51"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" s="51"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="51"/>
       <c r="B10" s="51"/>
       <c r="C10" s="51"/>
@@ -4554,8 +4584,9 @@
       <c r="E10" s="51"/>
       <c r="F10" s="51"/>
       <c r="G10" s="51"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10" s="51"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="51"/>
       <c r="B11" s="51"/>
       <c r="C11" s="51"/>
@@ -4563,18 +4594,18 @@
       <c r="E11" s="51"/>
       <c r="F11" s="51"/>
       <c r="G11" s="51"/>
+      <c r="H11" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
-      <formula1>"?, ATDL, DFF"</formula1>
+      <formula1>"?, ATDL"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4630,367 +4661,367 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -5003,11 +5034,348 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.7109375" customWidth="1"/>
+    <col min="2" max="2" width="37.42578125" customWidth="1"/>
+    <col min="3" max="3" width="32.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="44"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="53" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="5"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D4" s="5"/>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="B6" s="52" t="s">
+        <v>258</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="E6" s="24" t="s">
+        <v>158</v>
+      </c>
+      <c r="F6" s="24" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="51"/>
+      <c r="B7" s="51"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
+      <c r="F7" s="51"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="51"/>
+      <c r="B8" s="51"/>
+      <c r="C8" s="51"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="51"/>
+      <c r="F8" s="51"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="51"/>
+      <c r="B9" s="51"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="51"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="51"/>
+      <c r="B10" s="51"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="51"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="51"/>
+      <c r="B11" s="51"/>
+      <c r="C11" s="51"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="51"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+      <formula1>"?, DFF"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF00B0F0"/>
+  </sheetPr>
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.7109375" customWidth="1"/>
+    <col min="2" max="2" width="37.42578125" customWidth="1"/>
+    <col min="3" max="3" width="32.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="44"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="53" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="5"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D4" s="5"/>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="B6" s="52" t="s">
+        <v>110</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="E6" s="24" t="s">
+        <v>158</v>
+      </c>
+      <c r="F6" s="24" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="51"/>
+      <c r="B7" s="51"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
+      <c r="F7" s="51"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="51"/>
+      <c r="B8" s="51"/>
+      <c r="C8" s="51"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="51"/>
+      <c r="F8" s="51"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="51"/>
+      <c r="B9" s="51"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="51"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="51"/>
+      <c r="B10" s="51"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="51"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="51"/>
+      <c r="B11" s="51"/>
+      <c r="C11" s="51"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="51"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+      <formula1>"?, Generic"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF00B0F0"/>
+  </sheetPr>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomLeft" activeCell="I37" sqref="I37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" customWidth="1"/>
+    <col min="9" max="9" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" s="58"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="58"/>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>260</v>
+      </c>
+      <c r="D5" s="24" t="s">
+        <v>259</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="F5" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="G5" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="H5" s="24" t="s">
+        <v>114</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:H3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF00B0F0"/>
+  </sheetPr>
+  <dimension ref="A1:I5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5026,7 +5394,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="10" t="s">
-        <v>114</v>
+        <v>256</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -5036,43 +5404,43 @@
       <c r="A3" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="B3" s="57"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="57"/>
-      <c r="I3" s="57"/>
+      <c r="B3" s="58"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="58"/>
+      <c r="I3" s="58"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F5" s="24" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G5" s="24" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H5" s="24" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I5" s="24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -5109,15 +5477,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
@@ -5130,7 +5498,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -5145,7 +5513,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>1</v>
@@ -5163,7 +5531,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>24</v>
@@ -5178,7 +5546,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>24</v>
@@ -5211,13 +5579,13 @@
         <v>7</v>
       </c>
       <c r="E8" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="F8" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="F8" s="24" t="s">
+      <c r="G8" s="24" t="s">
         <v>140</v>
-      </c>
-      <c r="G8" s="24" t="s">
-        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -5268,23 +5636,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>124</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>125</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5" t="s">
@@ -5293,10 +5661,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>126</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>127</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5" t="s">
@@ -5305,10 +5673,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
@@ -5320,7 +5688,7 @@
         <v>86</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5" t="s">
@@ -5332,7 +5700,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5" t="s">
@@ -5350,22 +5718,22 @@
         <v>5</v>
       </c>
       <c r="C9" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="D9" s="23" t="s">
         <v>129</v>
-      </c>
-      <c r="D9" s="23" t="s">
-        <v>130</v>
       </c>
       <c r="E9" s="23" t="s">
         <v>7</v>
       </c>
       <c r="F9" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="G9" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="G9" s="24" t="s">
+      <c r="H9" s="24" t="s">
         <v>140</v>
-      </c>
-      <c r="H9" s="24" t="s">
-        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -5420,21 +5788,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -5445,7 +5813,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>13</v>
@@ -5459,7 +5827,7 @@
         <v>23</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>24</v>
@@ -5494,16 +5862,16 @@
         <v>15</v>
       </c>
       <c r="F8" s="24" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G8" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="H8" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="H8" s="24" t="s">
+      <c r="I8" s="24" t="s">
         <v>140</v>
-      </c>
-      <c r="I8" s="24" t="s">
-        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -5556,21 +5924,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>16</v>
@@ -5582,7 +5950,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>17</v>
@@ -5597,7 +5965,7 @@
         <v>23</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
@@ -5634,16 +6002,16 @@
         <v>15</v>
       </c>
       <c r="F8" s="24" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G8" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="H8" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="H8" s="24" t="s">
+      <c r="I8" s="24" t="s">
         <v>140</v>
-      </c>
-      <c r="I8" s="24" t="s">
-        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -5694,23 +6062,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="53"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>18</v>
@@ -5722,7 +6090,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>19</v>
@@ -5737,7 +6105,7 @@
         <v>23</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
@@ -5761,7 +6129,7 @@
         <v>21</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5" t="s">
@@ -5773,7 +6141,7 @@
         <v>22</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5" t="s">
@@ -5806,16 +6174,16 @@
         <v>27</v>
       </c>
       <c r="H10" s="24" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I10" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="J10" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="J10" s="24" t="s">
+      <c r="K10" s="24" t="s">
         <v>140</v>
-      </c>
-      <c r="K10" s="24" t="s">
-        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -5878,7 +6246,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>18</v>
@@ -5890,10 +6258,10 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5" t="s">
@@ -5902,10 +6270,10 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
@@ -5917,7 +6285,7 @@
         <v>33</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5" t="s">
@@ -5960,13 +6328,13 @@
         <v>31</v>
       </c>
       <c r="H9" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="I9" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="I9" s="24" t="s">
+      <c r="J9" s="24" t="s">
         <v>140</v>
-      </c>
-      <c r="J9" s="24" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated formatting on atom-type spreadsheets
</commit_message>
<xml_diff>
--- a/Atomistic-Class1/WebFF-Class1-DataTemplate.xlsx
+++ b/Atomistic-Class1/WebFF-Class1-DataTemplate.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\Projects\WebFF-Documentation\Atomistic-Class1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Projects\WebFF-Documentation\Atomistic-Class1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="18195" windowHeight="8190" firstSheet="28" activeTab="32"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="18195" windowHeight="8190" firstSheet="29" activeTab="28"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="20" r:id="rId1"/>
@@ -45,6 +45,7 @@
     <sheet name="AtomType-Generic" sheetId="38" r:id="rId31"/>
     <sheet name="Atom-Attributes-DFF" sheetId="41" r:id="rId32"/>
     <sheet name="Atom-Attributes-Generic" sheetId="31" r:id="rId33"/>
+    <sheet name="RelationTree-DFF" sheetId="43" r:id="rId34"/>
   </sheets>
   <definedNames>
     <definedName name="KeywordListTab_1" localSheetId="2">KeywordsList!$A$2:$A$74</definedName>
@@ -67,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="264">
   <si>
     <t>Harmonic</t>
   </si>
@@ -837,9 +838,6 @@
     <t>Nomenclature</t>
   </si>
   <si>
-    <t>Atom-Types-Generic</t>
-  </si>
-  <si>
     <t>DFF</t>
   </si>
   <si>
@@ -850,13 +848,25 @@
   </si>
   <si>
     <t>Coordination</t>
+  </si>
+  <si>
+    <t>Atom-Attributes-Generic</t>
+  </si>
+  <si>
+    <t>Atom-Attributes-DFF</t>
+  </si>
+  <si>
+    <t>RelationTree-DFF</t>
+  </si>
+  <si>
+    <t>RelationTree</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -933,6 +943,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -983,7 +1000,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -1147,6 +1164,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1158,7 +1184,7 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1255,6 +1281,13 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1611,91 +1644,91 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B14"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" style="31" customWidth="1"/>
+    <col min="1" max="1" width="18.59765625" style="31" customWidth="1"/>
     <col min="2" max="2" width="52" style="31" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="31"/>
+    <col min="3" max="16384" width="9.1328125" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="30" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:2" s="30" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A1" s="53" t="s">
         <v>122</v>
       </c>
       <c r="B1" s="53"/>
     </row>
-    <row r="2" spans="1:2" s="30" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" s="30" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="13"/>
       <c r="B2"/>
     </row>
-    <row r="3" spans="1:2" s="30" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" s="30" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="22" t="s">
         <v>97</v>
       </c>
       <c r="B3" s="38"/>
     </row>
-    <row r="4" spans="1:2" s="30" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" s="30" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="14"/>
       <c r="B4" s="18"/>
     </row>
-    <row r="5" spans="1:2" ht="22.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="22.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A5" s="32" t="s">
         <v>47</v>
       </c>
       <c r="B5" s="34"/>
     </row>
-    <row r="6" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="26" t="s">
         <v>45</v>
       </c>
       <c r="B6" s="37"/>
     </row>
-    <row r="7" spans="1:2" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="32.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="26" t="s">
         <v>46</v>
       </c>
       <c r="B7" s="35"/>
     </row>
-    <row r="8" spans="1:2" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="133.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="26" t="s">
         <v>67</v>
       </c>
       <c r="B8" s="36"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" s="33" t="s">
         <v>69</v>
       </c>
       <c r="B9" s="37"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" s="33" t="s">
         <v>70</v>
       </c>
       <c r="B10" s="37"/>
     </row>
-    <row r="11" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="33" t="s">
         <v>71</v>
       </c>
       <c r="B11" s="35"/>
     </row>
-    <row r="12" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="28" t="s">
         <v>68</v>
       </c>
       <c r="B12" s="37"/>
     </row>
-    <row r="13" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="28" t="s">
         <v>72</v>
       </c>
       <c r="B13" s="37"/>
     </row>
-    <row r="14" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="28" t="s">
         <v>73</v>
       </c>
@@ -1727,23 +1760,23 @@
       <selection pane="bottomLeft" activeCell="J25" sqref="A9:J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.265625" customWidth="1"/>
+    <col min="2" max="2" width="18.86328125" customWidth="1"/>
     <col min="3" max="4" width="16" customWidth="1"/>
     <col min="5" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" customWidth="1"/>
-    <col min="8" max="8" width="34.42578125" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.1328125" customWidth="1"/>
+    <col min="8" max="8" width="34.3984375" customWidth="1"/>
+    <col min="9" max="9" width="10.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:10" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>123</v>
       </c>
@@ -1755,7 +1788,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>125</v>
       </c>
@@ -1767,7 +1800,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>142</v>
       </c>
@@ -1779,7 +1812,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>33</v>
       </c>
@@ -1791,8 +1824,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="8" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" s="23" t="s">
         <v>4</v>
       </c>
@@ -1862,23 +1895,23 @@
       <selection pane="bottomLeft" activeCell="K27" sqref="A10:K27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.265625" customWidth="1"/>
+    <col min="2" max="2" width="18.86328125" customWidth="1"/>
     <col min="3" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" customWidth="1"/>
-    <col min="7" max="7" width="34.42578125" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="16.1328125" customWidth="1"/>
+    <col min="7" max="7" width="34.3984375" customWidth="1"/>
+    <col min="8" max="8" width="10.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>123</v>
       </c>
@@ -1890,7 +1923,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>125</v>
       </c>
@@ -1902,7 +1935,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>142</v>
       </c>
@@ -1914,7 +1947,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>33</v>
       </c>
@@ -1926,7 +1959,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>32</v>
       </c>
@@ -1938,8 +1971,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="9" spans="1:9" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="23" t="s">
         <v>4</v>
       </c>
@@ -2003,25 +2036,25 @@
       <selection pane="bottomLeft" activeCell="I32" sqref="A9:I32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.265625" customWidth="1"/>
+    <col min="2" max="2" width="18.86328125" customWidth="1"/>
+    <col min="3" max="3" width="17.86328125" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="7" width="18" customWidth="1"/>
-    <col min="8" max="8" width="16.140625" customWidth="1"/>
-    <col min="9" max="9" width="34.42578125" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" customWidth="1"/>
-    <col min="11" max="11" width="9.5703125" customWidth="1"/>
+    <col min="8" max="8" width="16.1328125" customWidth="1"/>
+    <col min="9" max="9" width="34.3984375" customWidth="1"/>
+    <col min="10" max="10" width="10.73046875" customWidth="1"/>
+    <col min="11" max="11" width="9.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:11" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>123</v>
       </c>
@@ -2033,7 +2066,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>125</v>
       </c>
@@ -2045,7 +2078,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>142</v>
       </c>
@@ -2057,7 +2090,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>143</v>
       </c>
@@ -2069,8 +2102,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="8" spans="1:11" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" s="23" t="s">
         <v>4</v>
       </c>
@@ -2137,24 +2170,24 @@
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.265625" customWidth="1"/>
+    <col min="2" max="2" width="18.86328125" customWidth="1"/>
+    <col min="3" max="3" width="17.86328125" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="7" width="18" customWidth="1"/>
-    <col min="8" max="9" width="16.140625" customWidth="1"/>
-    <col min="10" max="10" width="34.42578125" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" customWidth="1"/>
+    <col min="8" max="9" width="16.1328125" customWidth="1"/>
+    <col min="10" max="10" width="34.3984375" customWidth="1"/>
+    <col min="11" max="11" width="10.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:12" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>123</v>
       </c>
@@ -2166,7 +2199,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>125</v>
       </c>
@@ -2178,7 +2211,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>142</v>
       </c>
@@ -2190,7 +2223,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>143</v>
       </c>
@@ -2202,7 +2235,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
@@ -2271,19 +2304,19 @@
       <selection activeCell="A23" sqref="A10:T23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="19" width="16.28515625" customWidth="1"/>
-    <col min="20" max="20" width="33.7109375" customWidth="1"/>
-    <col min="21" max="22" width="10.7109375" customWidth="1"/>
+    <col min="1" max="19" width="16.265625" customWidth="1"/>
+    <col min="20" max="20" width="33.73046875" customWidth="1"/>
+    <col min="21" max="22" width="10.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:22" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>123</v>
       </c>
@@ -2295,7 +2328,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>125</v>
       </c>
@@ -2307,7 +2340,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>142</v>
       </c>
@@ -2319,7 +2352,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>143</v>
       </c>
@@ -2331,7 +2364,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>155</v>
       </c>
@@ -2343,8 +2376,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:22" s="48" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="9" spans="1:22" s="48" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="46" t="s">
         <v>4</v>
       </c>
@@ -2412,7 +2445,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:22" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7">
@@ -2447,18 +2480,18 @@
       <selection pane="bottomLeft" activeCell="M29" sqref="A9:M29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" style="7" customWidth="1"/>
+    <col min="1" max="1" width="16.265625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="18.86328125" style="7" customWidth="1"/>
     <col min="3" max="4" width="16" style="7" customWidth="1"/>
     <col min="5" max="5" width="18" style="6" customWidth="1"/>
     <col min="6" max="6" width="18" style="8" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" style="8" customWidth="1"/>
-    <col min="8" max="8" width="34.42578125" customWidth="1"/>
+    <col min="7" max="7" width="16.1328125" style="8" customWidth="1"/>
+    <col min="8" max="8" width="34.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:10" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="1" t="s">
         <v>57</v>
       </c>
@@ -2469,7 +2502,7 @@
       <c r="F1"/>
       <c r="G1"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2"/>
       <c r="B2"/>
       <c r="C2"/>
@@ -2478,7 +2511,7 @@
       <c r="F2"/>
       <c r="G2"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>123</v>
       </c>
@@ -2493,7 +2526,7 @@
       <c r="F3"/>
       <c r="G3"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>125</v>
       </c>
@@ -2508,7 +2541,7 @@
       <c r="F4"/>
       <c r="G4"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>142</v>
       </c>
@@ -2523,7 +2556,7 @@
       <c r="F5"/>
       <c r="G5"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>53</v>
       </c>
@@ -2538,7 +2571,7 @@
       <c r="F6"/>
       <c r="G6"/>
     </row>
-    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A7"/>
       <c r="B7"/>
       <c r="C7"/>
@@ -2547,7 +2580,7 @@
       <c r="F7"/>
       <c r="G7"/>
     </row>
-    <row r="8" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" s="23" t="s">
         <v>4</v>
       </c>
@@ -2579,7 +2612,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" s="50"/>
       <c r="B9" s="50"/>
       <c r="C9" s="50"/>
@@ -2587,7 +2620,7 @@
       <c r="F9" s="50"/>
       <c r="G9" s="50"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" s="50"/>
       <c r="B10" s="50"/>
       <c r="C10" s="50"/>
@@ -2595,7 +2628,7 @@
       <c r="F10" s="50"/>
       <c r="G10" s="50"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" s="50"/>
       <c r="B11" s="50"/>
       <c r="C11" s="50"/>
@@ -2603,7 +2636,7 @@
       <c r="F11" s="50"/>
       <c r="G11" s="50"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" s="50"/>
       <c r="B12" s="50"/>
       <c r="C12" s="50"/>
@@ -2611,7 +2644,7 @@
       <c r="F12" s="50"/>
       <c r="G12" s="50"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A13" s="50"/>
       <c r="B13" s="50"/>
       <c r="C13" s="50"/>
@@ -2657,17 +2690,17 @@
       <selection pane="bottomLeft" activeCell="L33" sqref="A10:L33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" style="7" customWidth="1"/>
+    <col min="1" max="1" width="16.265625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="18.86328125" style="7" customWidth="1"/>
     <col min="3" max="4" width="16" style="7" customWidth="1"/>
     <col min="5" max="5" width="18" style="6" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="34.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16.1328125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="34.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="1" t="s">
         <v>57</v>
       </c>
@@ -2677,7 +2710,7 @@
       <c r="E1"/>
       <c r="F1"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2"/>
       <c r="B2"/>
       <c r="C2"/>
@@ -2685,7 +2718,7 @@
       <c r="E2"/>
       <c r="F2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>123</v>
       </c>
@@ -2699,7 +2732,7 @@
       <c r="E3"/>
       <c r="F3"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>125</v>
       </c>
@@ -2713,7 +2746,7 @@
       <c r="E4"/>
       <c r="F4"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>142</v>
       </c>
@@ -2727,7 +2760,7 @@
       <c r="E5"/>
       <c r="F5"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>53</v>
       </c>
@@ -2741,7 +2774,7 @@
       <c r="E6"/>
       <c r="F6"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>54</v>
       </c>
@@ -2755,7 +2788,7 @@
       <c r="E7"/>
       <c r="F7"/>
     </row>
-    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8"/>
       <c r="B8"/>
       <c r="C8"/>
@@ -2763,7 +2796,7 @@
       <c r="E8"/>
       <c r="F8"/>
     </row>
-    <row r="9" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="23" t="s">
         <v>4</v>
       </c>
@@ -2792,31 +2825,31 @@
         <v>140</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" s="50"/>
       <c r="B10" s="50"/>
       <c r="C10" s="50"/>
       <c r="D10" s="50"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" s="50"/>
       <c r="B11" s="50"/>
       <c r="C11" s="50"/>
       <c r="D11" s="50"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" s="50"/>
       <c r="B12" s="50"/>
       <c r="C12" s="50"/>
       <c r="D12" s="50"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" s="50"/>
       <c r="B13" s="50"/>
       <c r="C13" s="50"/>
       <c r="D13" s="50"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" s="50"/>
       <c r="B14" s="50"/>
       <c r="C14" s="50"/>
@@ -2857,22 +2890,22 @@
       <selection pane="bottomLeft" activeCell="M35" sqref="A10:M35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.265625" customWidth="1"/>
+    <col min="2" max="2" width="18.86328125" customWidth="1"/>
     <col min="3" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" customWidth="1"/>
-    <col min="7" max="7" width="34.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16.1328125" customWidth="1"/>
+    <col min="7" max="7" width="34.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>123</v>
       </c>
@@ -2884,7 +2917,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>125</v>
       </c>
@@ -2896,7 +2929,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>142</v>
       </c>
@@ -2908,7 +2941,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>53</v>
       </c>
@@ -2920,7 +2953,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>54</v>
       </c>
@@ -2932,8 +2965,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="9" spans="1:9" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="23" t="s">
         <v>4</v>
       </c>
@@ -2997,23 +3030,23 @@
       <selection pane="bottomLeft" activeCell="I33" sqref="A9:I33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.265625" customWidth="1"/>
+    <col min="2" max="2" width="18.86328125" customWidth="1"/>
+    <col min="3" max="3" width="17.86328125" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="7" width="18" customWidth="1"/>
-    <col min="8" max="8" width="16.140625" customWidth="1"/>
-    <col min="9" max="9" width="34.42578125" customWidth="1"/>
+    <col min="8" max="8" width="16.1328125" customWidth="1"/>
+    <col min="9" max="9" width="34.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:11" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>123</v>
       </c>
@@ -3025,7 +3058,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>125</v>
       </c>
@@ -3037,7 +3070,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>142</v>
       </c>
@@ -3049,7 +3082,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>53</v>
       </c>
@@ -3061,8 +3094,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="8" spans="1:11" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" s="23" t="s">
         <v>4</v>
       </c>
@@ -3129,23 +3162,23 @@
       <selection pane="bottomLeft" activeCell="K29" sqref="A10:K29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.265625" customWidth="1"/>
+    <col min="2" max="2" width="18.86328125" customWidth="1"/>
     <col min="3" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" customWidth="1"/>
-    <col min="7" max="7" width="35.5703125" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16.1328125" customWidth="1"/>
+    <col min="7" max="7" width="35.59765625" customWidth="1"/>
+    <col min="8" max="8" width="10.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>123</v>
       </c>
@@ -3157,7 +3190,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>125</v>
       </c>
@@ -3169,7 +3202,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>142</v>
       </c>
@@ -3181,7 +3214,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>53</v>
       </c>
@@ -3193,7 +3226,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>66</v>
       </c>
@@ -3205,8 +3238,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="9" spans="1:9" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="23" t="s">
         <v>4</v>
       </c>
@@ -3267,36 +3300,36 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6:A27"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="25.140625" customWidth="1"/>
-    <col min="2" max="2" width="43.140625" customWidth="1"/>
+    <col min="1" max="1" width="25.1328125" customWidth="1"/>
+    <col min="2" max="2" width="43.1328125" customWidth="1"/>
     <col min="3" max="16384" width="9" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="54" t="s">
         <v>48</v>
       </c>
       <c r="B1" s="54"/>
     </row>
-    <row r="2" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="13"/>
     </row>
-    <row r="3" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="22" t="s">
         <v>97</v>
       </c>
       <c r="B3" s="12"/>
     </row>
-    <row r="4" spans="1:2" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="14"/>
       <c r="B4" s="18"/>
     </row>
-    <row r="5" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="23" t="s">
         <v>48</v>
       </c>
@@ -3304,71 +3337,71 @@
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" s="19"/>
       <c r="B6" s="19"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" s="19"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" s="19"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" s="19"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" s="19"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" s="19"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" s="19"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" s="19"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" s="19"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" s="19"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" s="19"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" s="19"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" s="19"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" s="19"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20" s="19"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A21" s="19"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A22" s="19"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A23" s="19"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A24" s="19"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A25" s="19"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A26" s="19"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A27" s="19"/>
     </row>
   </sheetData>
@@ -3403,24 +3436,24 @@
       <selection activeCell="I32" sqref="F19:I32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.265625" customWidth="1"/>
+    <col min="2" max="2" width="18.86328125" customWidth="1"/>
     <col min="3" max="4" width="16" customWidth="1"/>
     <col min="5" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" customWidth="1"/>
-    <col min="8" max="8" width="34.42578125" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.1328125" customWidth="1"/>
+    <col min="8" max="8" width="34.3984375" customWidth="1"/>
+    <col min="9" max="9" width="10.73046875" customWidth="1"/>
     <col min="10" max="10" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:10" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>123</v>
       </c>
@@ -3432,7 +3465,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>125</v>
       </c>
@@ -3444,7 +3477,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>142</v>
       </c>
@@ -3456,7 +3489,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>33</v>
       </c>
@@ -3468,7 +3501,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>32</v>
       </c>
@@ -3480,8 +3513,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="9" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="23" t="s">
         <v>4</v>
       </c>
@@ -3547,15 +3580,15 @@
       <selection pane="bottomLeft" activeCell="H23" sqref="A10:H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="35.85546875" customWidth="1"/>
+    <col min="2" max="2" width="35.86328125" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="36.140625" customWidth="1"/>
+    <col min="4" max="4" width="36.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="10" t="s">
         <v>74</v>
       </c>
@@ -3563,7 +3596,7 @@
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>123</v>
       </c>
@@ -3574,7 +3607,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>125</v>
       </c>
@@ -3585,7 +3618,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>82</v>
       </c>
@@ -3596,7 +3629,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>83</v>
       </c>
@@ -3607,7 +3640,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>156</v>
       </c>
@@ -3618,8 +3651,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="9" spans="1:6" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="23" t="s">
         <v>77</v>
       </c>
@@ -3674,15 +3707,15 @@
       <selection pane="bottomLeft" activeCell="I37" sqref="A10:I37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="32.85546875" customWidth="1"/>
+    <col min="2" max="2" width="32.86328125" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="36.140625" customWidth="1"/>
+    <col min="4" max="4" width="36.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="10" t="s">
         <v>74</v>
       </c>
@@ -3690,7 +3723,7 @@
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>123</v>
       </c>
@@ -3701,7 +3734,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>125</v>
       </c>
@@ -3712,7 +3745,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>82</v>
       </c>
@@ -3723,7 +3756,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>84</v>
       </c>
@@ -3734,7 +3767,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>156</v>
       </c>
@@ -3745,8 +3778,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="9" spans="1:6" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="23" t="s">
         <v>77</v>
       </c>
@@ -3801,15 +3834,15 @@
       <selection pane="bottomLeft" activeCell="J35" sqref="A10:J35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="32.85546875" customWidth="1"/>
+    <col min="2" max="2" width="32.86328125" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="36.140625" customWidth="1"/>
+    <col min="4" max="4" width="36.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="53" t="s">
         <v>74</v>
       </c>
@@ -3819,7 +3852,7 @@
       <c r="E1" s="53"/>
       <c r="F1" s="53"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>123</v>
       </c>
@@ -3830,7 +3863,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>125</v>
       </c>
@@ -3841,7 +3874,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>86</v>
       </c>
@@ -3852,7 +3885,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>88</v>
       </c>
@@ -3863,7 +3896,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>156</v>
       </c>
@@ -3874,8 +3907,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="9" spans="1:6" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="23" t="s">
         <v>77</v>
       </c>
@@ -3933,15 +3966,15 @@
       <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="37.42578125" customWidth="1"/>
+    <col min="2" max="2" width="37.3984375" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="36.140625" customWidth="1"/>
+    <col min="4" max="4" width="36.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="10" t="s">
         <v>74</v>
       </c>
@@ -3949,7 +3982,7 @@
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>123</v>
       </c>
@@ -3960,7 +3993,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>125</v>
       </c>
@@ -3971,7 +4004,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>82</v>
       </c>
@@ -3982,7 +4015,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>83</v>
       </c>
@@ -3993,7 +4026,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>156</v>
       </c>
@@ -4004,8 +4037,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="9" spans="1:6" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="23" t="s">
         <v>77</v>
       </c>
@@ -4060,16 +4093,16 @@
       <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="35.7109375" customWidth="1"/>
+    <col min="2" max="2" width="35.73046875" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" customWidth="1"/>
-    <col min="5" max="5" width="33.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.59765625" customWidth="1"/>
+    <col min="5" max="5" width="33.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="53" t="s">
         <v>74</v>
       </c>
@@ -4080,7 +4113,7 @@
       <c r="F1" s="53"/>
       <c r="G1" s="53"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>123</v>
       </c>
@@ -4091,7 +4124,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>125</v>
       </c>
@@ -4102,7 +4135,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>82</v>
       </c>
@@ -4113,7 +4146,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>83</v>
       </c>
@@ -4124,7 +4157,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>156</v>
       </c>
@@ -4135,8 +4168,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="9" spans="1:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="23" t="s">
         <v>4</v>
       </c>
@@ -4196,16 +4229,16 @@
       <selection activeCell="L35" sqref="A6:L35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="12.140625" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" customWidth="1"/>
-    <col min="7" max="7" width="26.28515625" customWidth="1"/>
+    <col min="1" max="1" width="12.1328125" customWidth="1"/>
+    <col min="2" max="2" width="11.59765625" customWidth="1"/>
+    <col min="7" max="7" width="26.265625" customWidth="1"/>
     <col min="8" max="8" width="11" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" customWidth="1"/>
+    <col min="9" max="9" width="16.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="53" t="s">
         <v>95</v>
       </c>
@@ -4218,7 +4251,7 @@
       <c r="H1" s="53"/>
       <c r="I1" s="53"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="9" t="s">
         <v>97</v>
       </c>
@@ -4233,8 +4266,8 @@
       <c r="H3" s="56"/>
       <c r="I3" s="57"/>
     </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="5" spans="1:9" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="23" t="s">
         <v>77</v>
       </c>
@@ -4284,22 +4317,22 @@
       <selection activeCell="K30" sqref="A6:K30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="12.140625" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" customWidth="1"/>
-    <col min="8" max="9" width="15.7109375" customWidth="1"/>
-    <col min="10" max="10" width="18.140625" customWidth="1"/>
-    <col min="11" max="11" width="26.28515625" customWidth="1"/>
+    <col min="1" max="1" width="12.1328125" customWidth="1"/>
+    <col min="2" max="2" width="11.59765625" customWidth="1"/>
+    <col min="3" max="3" width="15.1328125" customWidth="1"/>
+    <col min="5" max="5" width="10.3984375" customWidth="1"/>
+    <col min="6" max="6" width="11.265625" customWidth="1"/>
+    <col min="7" max="7" width="12.1328125" customWidth="1"/>
+    <col min="8" max="9" width="15.73046875" customWidth="1"/>
+    <col min="10" max="10" width="18.1328125" customWidth="1"/>
+    <col min="11" max="11" width="26.265625" customWidth="1"/>
     <col min="12" max="12" width="11" customWidth="1"/>
-    <col min="13" max="13" width="16.7109375" customWidth="1"/>
+    <col min="13" max="13" width="16.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:13" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="53" t="s">
         <v>130</v>
       </c>
@@ -4316,7 +4349,7 @@
       <c r="L1" s="53"/>
       <c r="M1" s="53"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" s="9" t="s">
         <v>97</v>
       </c>
@@ -4335,8 +4368,8 @@
       <c r="L3" s="56"/>
       <c r="M3" s="57"/>
     </row>
-    <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="5" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="23" t="s">
         <v>77</v>
       </c>
@@ -4397,17 +4430,17 @@
       <selection activeCell="M34" sqref="A6:M34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.86328125" customWidth="1"/>
+    <col min="3" max="3" width="10.1328125" customWidth="1"/>
+    <col min="4" max="4" width="9.73046875" customWidth="1"/>
+    <col min="5" max="5" width="22.265625" customWidth="1"/>
+    <col min="6" max="6" width="11.3984375" customWidth="1"/>
+    <col min="7" max="7" width="15.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="53" t="s">
         <v>99</v>
       </c>
@@ -4420,7 +4453,7 @@
       <c r="H1" s="10"/>
       <c r="I1" s="10"/>
     </row>
-    <row r="3" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="11" t="s">
         <v>97</v>
       </c>
@@ -4431,8 +4464,8 @@
       <c r="F3" s="42"/>
       <c r="G3" s="43"/>
     </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="5" spans="1:9" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="23" t="s">
         <v>100</v>
       </c>
@@ -4470,22 +4503,22 @@
   </sheetPr>
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" customWidth="1"/>
-    <col min="2" max="2" width="37.42578125" customWidth="1"/>
+    <col min="1" max="1" width="28.73046875" customWidth="1"/>
+    <col min="2" max="2" width="37.3984375" customWidth="1"/>
     <col min="3" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="35.28515625" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="44"/>
+    <col min="5" max="5" width="35.265625" customWidth="1"/>
+    <col min="7" max="7" width="15.73046875" customWidth="1"/>
+    <col min="8" max="8" width="12.3984375" customWidth="1"/>
+    <col min="9" max="16384" width="9.1328125" style="44"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:8" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="53" t="s">
         <v>113</v>
       </c>
@@ -4497,7 +4530,7 @@
       <c r="G1" s="53"/>
       <c r="H1" s="53"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>255</v>
       </c>
@@ -4509,7 +4542,7 @@
       </c>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>138</v>
       </c>
@@ -4519,15 +4552,15 @@
       </c>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="6" spans="1:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A6" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="B6" s="52" t="s">
+      <c r="B6" s="59" t="s">
         <v>252</v>
       </c>
-      <c r="C6" s="52" t="s">
+      <c r="C6" s="59" t="s">
         <v>253</v>
       </c>
       <c r="D6" s="52" t="s">
@@ -4546,7 +4579,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="51"/>
       <c r="B7" s="51"/>
       <c r="C7" s="51"/>
@@ -4556,7 +4589,7 @@
       <c r="G7" s="51"/>
       <c r="H7" s="51"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="51"/>
       <c r="B8" s="51"/>
       <c r="C8" s="51"/>
@@ -4566,7 +4599,7 @@
       <c r="G8" s="51"/>
       <c r="H8" s="51"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" s="51"/>
       <c r="B9" s="51"/>
       <c r="C9" s="51"/>
@@ -4576,7 +4609,7 @@
       <c r="G9" s="51"/>
       <c r="H9" s="51"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" s="51"/>
       <c r="B10" s="51"/>
       <c r="C10" s="51"/>
@@ -4586,7 +4619,7 @@
       <c r="G10" s="51"/>
       <c r="H10" s="51"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" s="51"/>
       <c r="B11" s="51"/>
       <c r="C11" s="51"/>
@@ -4606,6 +4639,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4620,406 +4654,406 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="17" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="31" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="33" max="37" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.73046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.73046875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.59765625" bestFit="1" customWidth="1"/>
+    <col min="13" max="17" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.73046875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.86328125" bestFit="1" customWidth="1"/>
+    <col min="21" max="31" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="23.86328125" bestFit="1" customWidth="1"/>
+    <col min="33" max="37" width="8.3984375" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="14" bestFit="1" customWidth="1"/>
-    <col min="39" max="44" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="46" max="58" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="60" max="61" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="39" max="44" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="19.86328125" bestFit="1" customWidth="1"/>
+    <col min="46" max="58" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="6.59765625" bestFit="1" customWidth="1"/>
+    <col min="60" max="61" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="12.73046875" bestFit="1" customWidth="1"/>
     <col min="64" max="64" width="7" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="70" max="72" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="25.86328125" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="7.73046875" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="6.3984375" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="6.1328125" bestFit="1" customWidth="1"/>
+    <col min="70" max="72" width="8.3984375" bestFit="1" customWidth="1"/>
     <col min="73" max="73" width="25" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="9.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" s="7" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" s="7" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" s="7" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" s="7" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" s="7" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A7" s="7" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A8" s="7" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A9" s="7" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A10" s="7" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A11" s="7" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A12" s="7" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A13" s="7" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A14" s="7" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A15" s="7" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A16" s="7" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" s="7" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" s="7" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" s="7" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20" s="7" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A21" s="7" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A22" s="7" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A23" s="7" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A24" s="7" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A25" s="7" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A26" s="7" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A27" s="7" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A28" s="7" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A29" s="7" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A30" s="7" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A31" s="7" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A32" s="7" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A33" s="7" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A34" s="7" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A35" s="7" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A36" s="7" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A37" s="7" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A38" s="7" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A39" s="7" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A40" s="7" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A41" s="7" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A42" s="7" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A43" s="7" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A44" s="7" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A45" s="7" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A46" s="7" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A47" s="7" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A48" s="7" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A49" s="7" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A50" s="7" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A51" s="7" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A52" s="7" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A53" s="7" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A54" s="7" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A55" s="7" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A56" s="7" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A57" s="7" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A58" s="7" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A59" s="7" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A60" s="7" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A61" s="7" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A62" s="7" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A63" s="7" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A64" s="7" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A65" s="7" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A66" s="7" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A67" s="7" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A68" s="7" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A69" s="7" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A70" s="7" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A71" s="7" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A72" s="7" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A73" s="7" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A74" s="7" t="s">
         <v>193</v>
       </c>
@@ -5037,21 +5071,21 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" customWidth="1"/>
-    <col min="2" max="2" width="37.42578125" customWidth="1"/>
-    <col min="3" max="3" width="32.7109375" customWidth="1"/>
+    <col min="1" max="1" width="28.73046875" customWidth="1"/>
+    <col min="2" max="2" width="37.3984375" customWidth="1"/>
+    <col min="3" max="3" width="32.73046875" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="44"/>
+    <col min="5" max="5" width="16.73046875" customWidth="1"/>
+    <col min="6" max="6" width="12.3984375" customWidth="1"/>
+    <col min="7" max="16384" width="9.1328125" style="44"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="53" t="s">
         <v>113</v>
       </c>
@@ -5061,19 +5095,19 @@
       <c r="E1" s="53"/>
       <c r="F1" s="53"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>255</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>138</v>
       </c>
@@ -5083,13 +5117,13 @@
       </c>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="6" spans="1:6" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A6" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="B6" s="52" t="s">
-        <v>258</v>
+      <c r="B6" s="59" t="s">
+        <v>257</v>
       </c>
       <c r="C6" s="24" t="s">
         <v>46</v>
@@ -5104,7 +5138,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="51"/>
       <c r="B7" s="51"/>
       <c r="C7" s="51"/>
@@ -5112,7 +5146,7 @@
       <c r="E7" s="51"/>
       <c r="F7" s="51"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="51"/>
       <c r="B8" s="51"/>
       <c r="C8" s="51"/>
@@ -5120,7 +5154,7 @@
       <c r="E8" s="51"/>
       <c r="F8" s="51"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="51"/>
       <c r="B9" s="51"/>
       <c r="C9" s="51"/>
@@ -5128,7 +5162,7 @@
       <c r="E9" s="51"/>
       <c r="F9" s="51"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="51"/>
       <c r="B10" s="51"/>
       <c r="C10" s="51"/>
@@ -5136,7 +5170,7 @@
       <c r="E10" s="51"/>
       <c r="F10" s="51"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="51"/>
       <c r="B11" s="51"/>
       <c r="C11" s="51"/>
@@ -5165,21 +5199,21 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" customWidth="1"/>
-    <col min="2" max="2" width="37.42578125" customWidth="1"/>
-    <col min="3" max="3" width="32.7109375" customWidth="1"/>
+    <col min="1" max="1" width="28.73046875" customWidth="1"/>
+    <col min="2" max="2" width="37.3984375" customWidth="1"/>
+    <col min="3" max="3" width="32.73046875" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="44"/>
+    <col min="5" max="5" width="16.73046875" customWidth="1"/>
+    <col min="6" max="6" width="12.3984375" customWidth="1"/>
+    <col min="7" max="16384" width="9.1328125" style="44"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="53" t="s">
         <v>113</v>
       </c>
@@ -5189,7 +5223,7 @@
       <c r="E1" s="53"/>
       <c r="F1" s="53"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>255</v>
       </c>
@@ -5201,7 +5235,7 @@
       </c>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>138</v>
       </c>
@@ -5211,12 +5245,12 @@
       </c>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="6" spans="1:6" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A6" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="B6" s="52" t="s">
+      <c r="B6" s="59" t="s">
         <v>110</v>
       </c>
       <c r="C6" s="24" t="s">
@@ -5232,7 +5266,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="51"/>
       <c r="B7" s="51"/>
       <c r="C7" s="51"/>
@@ -5240,7 +5274,7 @@
       <c r="E7" s="51"/>
       <c r="F7" s="51"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="51"/>
       <c r="B8" s="51"/>
       <c r="C8" s="51"/>
@@ -5248,7 +5282,7 @@
       <c r="E8" s="51"/>
       <c r="F8" s="51"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="51"/>
       <c r="B9" s="51"/>
       <c r="C9" s="51"/>
@@ -5256,7 +5290,7 @@
       <c r="E9" s="51"/>
       <c r="F9" s="51"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="51"/>
       <c r="B10" s="51"/>
       <c r="C10" s="51"/>
@@ -5264,7 +5298,7 @@
       <c r="E10" s="51"/>
       <c r="F10" s="51"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="51"/>
       <c r="B11" s="51"/>
       <c r="C11" s="51"/>
@@ -5294,31 +5328,31 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I37" sqref="I37"/>
+      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.1328125" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.1328125" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" customWidth="1"/>
-    <col min="7" max="7" width="17.140625" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="14.59765625" customWidth="1"/>
+    <col min="7" max="7" width="17.1328125" customWidth="1"/>
+    <col min="8" max="8" width="17.73046875" customWidth="1"/>
     <col min="9" max="9" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:8" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="10" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="17" t="s">
         <v>97</v>
       </c>
@@ -5330,8 +5364,8 @@
       <c r="G3" s="58"/>
       <c r="H3" s="58"/>
     </row>
-    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="5" spans="1:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="23" t="s">
         <v>111</v>
       </c>
@@ -5339,10 +5373,10 @@
         <v>121</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E5" s="24" t="s">
         <v>118</v>
@@ -5373,34 +5407,34 @@
   </sheetPr>
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G31" sqref="G31"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.1328125" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.1328125" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" customWidth="1"/>
-    <col min="8" max="8" width="17.140625" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="14.59765625" customWidth="1"/>
+    <col min="7" max="7" width="13.3984375" customWidth="1"/>
+    <col min="8" max="8" width="17.1328125" customWidth="1"/>
+    <col min="9" max="9" width="17.73046875" customWidth="1"/>
     <col min="10" max="10" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="10" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="17" t="s">
         <v>97</v>
       </c>
@@ -5413,8 +5447,8 @@
       <c r="H3" s="58"/>
       <c r="I3" s="58"/>
     </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="5" spans="1:9" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="23" t="s">
         <v>111</v>
       </c>
@@ -5446,6 +5480,59 @@
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B3:I3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="3"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="18.59765625" style="31" customWidth="1"/>
+    <col min="2" max="2" width="52" style="31" customWidth="1"/>
+    <col min="3" max="16384" width="9.1328125" style="31"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="30" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A1" s="53" t="s">
+        <v>262</v>
+      </c>
+      <c r="B1" s="53"/>
+    </row>
+    <row r="2" spans="1:2" s="30" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="13"/>
+      <c r="B2"/>
+    </row>
+    <row r="3" spans="1:2" s="30" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" s="38"/>
+    </row>
+    <row r="4" spans="1:2" s="30" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A4" s="14"/>
+      <c r="B4" s="18"/>
+    </row>
+    <row r="5" spans="1:2" ht="338.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="60" t="s">
+        <v>263</v>
+      </c>
+      <c r="B5" s="61"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5464,19 +5551,19 @@
       <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.73046875" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" customWidth="1"/>
-    <col min="5" max="5" width="36.140625" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="40"/>
+    <col min="4" max="4" width="16.1328125" customWidth="1"/>
+    <col min="5" max="5" width="36.1328125" customWidth="1"/>
+    <col min="6" max="6" width="9.73046875" customWidth="1"/>
+    <col min="7" max="7" width="10.3984375" customWidth="1"/>
+    <col min="8" max="16384" width="9.1328125" style="40"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="53" t="s">
         <v>8</v>
       </c>
@@ -5487,7 +5574,7 @@
       <c r="F1" s="53"/>
       <c r="G1" s="53"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="13"/>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
@@ -5496,7 +5583,7 @@
       <c r="F2" s="15"/>
       <c r="G2" s="16"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>123</v>
       </c>
@@ -5511,7 +5598,7 @@
       <c r="F3" s="15"/>
       <c r="G3" s="16"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>125</v>
       </c>
@@ -5526,7 +5613,7 @@
       <c r="F4" s="15"/>
       <c r="G4" s="16"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
@@ -5541,7 +5628,7 @@
       <c r="F5" s="15"/>
       <c r="G5" s="16"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
@@ -5556,7 +5643,7 @@
       <c r="F6" s="15"/>
       <c r="G6" s="16"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A7" s="20"/>
       <c r="B7" s="20"/>
       <c r="C7" s="20"/>
@@ -5565,7 +5652,7 @@
       <c r="F7" s="20"/>
       <c r="G7" s="21"/>
     </row>
-    <row r="8" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" s="23" t="s">
         <v>4</v>
       </c>
@@ -5622,20 +5709,20 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" customWidth="1"/>
+    <col min="1" max="1" width="17.86328125" customWidth="1"/>
+    <col min="2" max="2" width="22.86328125" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
-    <col min="6" max="6" width="34.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.1328125" customWidth="1"/>
+    <col min="6" max="6" width="34.3984375" customWidth="1"/>
     <col min="7" max="7" width="9"/>
-    <col min="8" max="8" width="10.140625" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="39"/>
+    <col min="8" max="8" width="10.1328125" customWidth="1"/>
+    <col min="9" max="16384" width="9.1328125" style="39"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:8" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="53" t="s">
         <v>8</v>
       </c>
@@ -5647,7 +5734,7 @@
       <c r="G1" s="53"/>
       <c r="H1" s="53"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>123</v>
       </c>
@@ -5659,7 +5746,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>125</v>
       </c>
@@ -5671,7 +5758,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>127</v>
       </c>
@@ -5683,7 +5770,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>86</v>
       </c>
@@ -5695,7 +5782,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>3</v>
       </c>
@@ -5707,10 +5794,10 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B8" s="3"/>
     </row>
-    <row r="9" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="23" t="s">
         <v>4</v>
       </c>
@@ -5773,21 +5860,21 @@
       <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="1" max="1" width="16.73046875" customWidth="1"/>
+    <col min="2" max="2" width="20.265625" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" customWidth="1"/>
-    <col min="7" max="7" width="31.42578125" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="25"/>
+    <col min="5" max="5" width="16.1328125" customWidth="1"/>
+    <col min="6" max="6" width="14.3984375" customWidth="1"/>
+    <col min="7" max="7" width="31.3984375" customWidth="1"/>
+    <col min="8" max="8" width="11.1328125" customWidth="1"/>
+    <col min="9" max="9" width="11.265625" customWidth="1"/>
+    <col min="10" max="16384" width="9.1328125" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="53" t="s">
         <v>9</v>
       </c>
@@ -5800,7 +5887,7 @@
       <c r="H1" s="53"/>
       <c r="I1" s="53"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>123</v>
       </c>
@@ -5811,7 +5898,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>125</v>
       </c>
@@ -5822,7 +5909,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>23</v>
       </c>
@@ -5833,7 +5920,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
@@ -5844,8 +5931,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="8" spans="1:9" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" s="23" t="s">
         <v>4</v>
       </c>
@@ -5909,21 +5996,21 @@
       <selection pane="bottomLeft" activeCell="G32" sqref="A9:G32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.265625" customWidth="1"/>
+    <col min="2" max="2" width="18.86328125" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" customWidth="1"/>
-    <col min="7" max="7" width="34.42578125" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="27"/>
+    <col min="5" max="5" width="16.1328125" customWidth="1"/>
+    <col min="6" max="6" width="11.1328125" customWidth="1"/>
+    <col min="7" max="7" width="34.3984375" customWidth="1"/>
+    <col min="8" max="8" width="10.73046875" customWidth="1"/>
+    <col min="9" max="9" width="15.1328125" customWidth="1"/>
+    <col min="10" max="16384" width="9.1328125" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="53" t="s">
         <v>9</v>
       </c>
@@ -5936,7 +6023,7 @@
       <c r="H1" s="53"/>
       <c r="I1" s="53"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>123</v>
       </c>
@@ -5948,7 +6035,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>125</v>
       </c>
@@ -5960,7 +6047,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>23</v>
       </c>
@@ -5972,7 +6059,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
@@ -5984,8 +6071,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="8" spans="1:9" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" s="23" t="s">
         <v>4</v>
       </c>
@@ -6049,19 +6136,19 @@
       <selection pane="bottomLeft" activeCell="H27" sqref="A11:H27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.265625" customWidth="1"/>
+    <col min="2" max="2" width="18.86328125" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="7" width="16.140625" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" customWidth="1"/>
-    <col min="9" max="9" width="34.42578125" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" customWidth="1"/>
+    <col min="5" max="7" width="16.1328125" customWidth="1"/>
+    <col min="8" max="8" width="11.86328125" customWidth="1"/>
+    <col min="9" max="9" width="34.3984375" customWidth="1"/>
+    <col min="11" max="11" width="9.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:11" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="53" t="s">
         <v>9</v>
       </c>
@@ -6076,7 +6163,7 @@
       <c r="J1" s="53"/>
       <c r="K1" s="53"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>123</v>
       </c>
@@ -6088,7 +6175,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>125</v>
       </c>
@@ -6100,7 +6187,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>23</v>
       </c>
@@ -6112,7 +6199,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
@@ -6124,7 +6211,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>21</v>
       </c>
@@ -6136,7 +6223,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" s="4" t="s">
         <v>22</v>
       </c>
@@ -6148,10 +6235,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B9" s="3"/>
     </row>
-    <row r="10" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A10" s="23" t="s">
         <v>4</v>
       </c>
@@ -6227,24 +6314,24 @@
       <selection pane="bottomLeft" activeCell="H33" sqref="A10:H33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.265625" customWidth="1"/>
+    <col min="2" max="2" width="18.86328125" customWidth="1"/>
     <col min="3" max="4" width="16" customWidth="1"/>
     <col min="5" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" customWidth="1"/>
-    <col min="8" max="8" width="34.42578125" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.1328125" customWidth="1"/>
+    <col min="8" max="8" width="34.3984375" customWidth="1"/>
+    <col min="9" max="9" width="10.73046875" customWidth="1"/>
     <col min="10" max="10" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:10" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>123</v>
       </c>
@@ -6256,7 +6343,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>125</v>
       </c>
@@ -6268,7 +6355,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>142</v>
       </c>
@@ -6280,7 +6367,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>33</v>
       </c>
@@ -6292,7 +6379,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>32</v>
       </c>
@@ -6304,8 +6391,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="9" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="23" t="s">
         <v>4</v>
       </c>
@@ -6337,19 +6424,19 @@
         <v>140</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="F10" s="8"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="F11" s="8"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="F12" s="8"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="F13" s="8"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="F14" s="8"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Addition of Soft Potentials to the CG Excel template in addition to the implementation of a Relation Tree Python module for DFF
</commit_message>
<xml_diff>
--- a/Atomistic-Class1/WebFF-Class1-DataTemplate.xlsx
+++ b/Atomistic-Class1/WebFF-Class1-DataTemplate.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Projects\WebFF-Documentation\Atomistic-Class1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\Projects\WebFF-Documentation\Atomistic-Class1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="18195" windowHeight="8190" firstSheet="29" activeTab="28"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="18195" windowHeight="8190" firstSheet="28" activeTab="32"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="20" r:id="rId1"/>
@@ -1264,6 +1264,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1281,13 +1288,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1647,88 +1647,88 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.59765625" style="31" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" style="31" customWidth="1"/>
     <col min="2" max="2" width="52" style="31" customWidth="1"/>
-    <col min="3" max="16384" width="9.1328125" style="31"/>
+    <col min="3" max="16384" width="9.140625" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="30" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A1" s="53" t="s">
+    <row r="1" spans="1:2" s="30" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="56" t="s">
         <v>122</v>
       </c>
-      <c r="B1" s="53"/>
-    </row>
-    <row r="2" spans="1:2" s="30" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B1" s="56"/>
+    </row>
+    <row r="2" spans="1:2" s="30" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
       <c r="B2"/>
     </row>
-    <row r="3" spans="1:2" s="30" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" s="30" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
         <v>97</v>
       </c>
       <c r="B3" s="38"/>
     </row>
-    <row r="4" spans="1:2" s="30" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:2" s="30" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="14"/>
       <c r="B4" s="18"/>
     </row>
-    <row r="5" spans="1:2" ht="22.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" ht="22.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A5" s="32" t="s">
         <v>47</v>
       </c>
       <c r="B5" s="34"/>
     </row>
-    <row r="6" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
         <v>45</v>
       </c>
       <c r="B6" s="37"/>
     </row>
-    <row r="7" spans="1:2" ht="32.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
         <v>46</v>
       </c>
       <c r="B7" s="35"/>
     </row>
-    <row r="8" spans="1:2" ht="133.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" ht="133.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
         <v>67</v>
       </c>
       <c r="B8" s="36"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
         <v>69</v>
       </c>
       <c r="B9" s="37"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="33" t="s">
         <v>70</v>
       </c>
       <c r="B10" s="37"/>
     </row>
-    <row r="11" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="33" t="s">
         <v>71</v>
       </c>
       <c r="B11" s="35"/>
     </row>
-    <row r="12" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="28" t="s">
         <v>68</v>
       </c>
       <c r="B12" s="37"/>
     </row>
-    <row r="13" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="28" t="s">
         <v>72</v>
       </c>
       <c r="B13" s="37"/>
     </row>
-    <row r="14" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="28" t="s">
         <v>73</v>
       </c>
@@ -1760,23 +1760,23 @@
       <selection pane="bottomLeft" activeCell="J25" sqref="A9:J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.265625" customWidth="1"/>
-    <col min="2" max="2" width="18.86328125" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
     <col min="3" max="4" width="16" customWidth="1"/>
     <col min="5" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="16.1328125" customWidth="1"/>
-    <col min="8" max="8" width="34.3984375" customWidth="1"/>
-    <col min="9" max="9" width="10.73046875" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" customWidth="1"/>
+    <col min="8" max="8" width="34.42578125" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="30.75" x14ac:dyDescent="0.9">
+    <row r="1" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>123</v>
       </c>
@@ -1788,7 +1788,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>125</v>
       </c>
@@ -1800,7 +1800,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>142</v>
       </c>
@@ -1812,7 +1812,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>33</v>
       </c>
@@ -1824,8 +1824,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="8" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="23" t="s">
         <v>4</v>
       </c>
@@ -1895,23 +1895,23 @@
       <selection pane="bottomLeft" activeCell="K27" sqref="A10:K27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.265625" customWidth="1"/>
-    <col min="2" max="2" width="18.86328125" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
     <col min="3" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="16.1328125" customWidth="1"/>
-    <col min="7" max="7" width="34.3984375" customWidth="1"/>
-    <col min="8" max="8" width="10.73046875" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" customWidth="1"/>
+    <col min="7" max="7" width="34.42578125" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30.75" x14ac:dyDescent="0.9">
+    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>123</v>
       </c>
@@ -1923,7 +1923,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>125</v>
       </c>
@@ -1935,7 +1935,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>142</v>
       </c>
@@ -1947,7 +1947,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>33</v>
       </c>
@@ -1959,7 +1959,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>32</v>
       </c>
@@ -1971,8 +1971,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="9" spans="1:9" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
         <v>4</v>
       </c>
@@ -2036,25 +2036,25 @@
       <selection pane="bottomLeft" activeCell="I32" sqref="A9:I32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.265625" customWidth="1"/>
-    <col min="2" max="2" width="18.86328125" customWidth="1"/>
-    <col min="3" max="3" width="17.86328125" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="7" width="18" customWidth="1"/>
-    <col min="8" max="8" width="16.1328125" customWidth="1"/>
-    <col min="9" max="9" width="34.3984375" customWidth="1"/>
-    <col min="10" max="10" width="10.73046875" customWidth="1"/>
-    <col min="11" max="11" width="9.59765625" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" customWidth="1"/>
+    <col min="9" max="9" width="34.42578125" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" customWidth="1"/>
+    <col min="11" max="11" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30.75" x14ac:dyDescent="0.9">
+    <row r="1" spans="1:11" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>123</v>
       </c>
@@ -2066,7 +2066,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>125</v>
       </c>
@@ -2078,7 +2078,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>142</v>
       </c>
@@ -2090,7 +2090,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>143</v>
       </c>
@@ -2102,8 +2102,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="8" spans="1:11" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="23" t="s">
         <v>4</v>
       </c>
@@ -2170,24 +2170,24 @@
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.265625" customWidth="1"/>
-    <col min="2" max="2" width="18.86328125" customWidth="1"/>
-    <col min="3" max="3" width="17.86328125" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="7" width="18" customWidth="1"/>
-    <col min="8" max="9" width="16.1328125" customWidth="1"/>
-    <col min="10" max="10" width="34.3984375" customWidth="1"/>
-    <col min="11" max="11" width="10.73046875" customWidth="1"/>
+    <col min="8" max="9" width="16.140625" customWidth="1"/>
+    <col min="10" max="10" width="34.42578125" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="30.75" x14ac:dyDescent="0.9">
+    <row r="1" spans="1:12" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>123</v>
       </c>
@@ -2199,7 +2199,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>125</v>
       </c>
@@ -2211,7 +2211,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>142</v>
       </c>
@@ -2223,7 +2223,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>143</v>
       </c>
@@ -2235,7 +2235,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
@@ -2304,19 +2304,19 @@
       <selection activeCell="A23" sqref="A10:T23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="19" width="16.265625" customWidth="1"/>
-    <col min="20" max="20" width="33.73046875" customWidth="1"/>
-    <col min="21" max="22" width="10.73046875" customWidth="1"/>
+    <col min="1" max="19" width="16.28515625" customWidth="1"/>
+    <col min="20" max="20" width="33.7109375" customWidth="1"/>
+    <col min="21" max="22" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="30.75" x14ac:dyDescent="0.9">
+    <row r="1" spans="1:22" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>123</v>
       </c>
@@ -2328,7 +2328,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>125</v>
       </c>
@@ -2340,7 +2340,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>142</v>
       </c>
@@ -2352,7 +2352,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>143</v>
       </c>
@@ -2364,7 +2364,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>155</v>
       </c>
@@ -2376,8 +2376,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="9" spans="1:22" s="48" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:22" s="48" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="46" t="s">
         <v>4</v>
       </c>
@@ -2445,7 +2445,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
+    <row r="10" spans="1:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7">
@@ -2480,18 +2480,18 @@
       <selection pane="bottomLeft" activeCell="M29" sqref="A9:M29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.265625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="18.86328125" style="7" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" style="7" customWidth="1"/>
     <col min="3" max="4" width="16" style="7" customWidth="1"/>
     <col min="5" max="5" width="18" style="6" customWidth="1"/>
     <col min="6" max="6" width="18" style="8" customWidth="1"/>
-    <col min="7" max="7" width="16.1328125" style="8" customWidth="1"/>
-    <col min="8" max="8" width="34.3984375" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" style="8" customWidth="1"/>
+    <col min="8" max="8" width="34.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="30.75" x14ac:dyDescent="0.9">
+    <row r="1" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>57</v>
       </c>
@@ -2502,7 +2502,7 @@
       <c r="F1"/>
       <c r="G1"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2"/>
       <c r="B2"/>
       <c r="C2"/>
@@ -2511,7 +2511,7 @@
       <c r="F2"/>
       <c r="G2"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>123</v>
       </c>
@@ -2526,7 +2526,7 @@
       <c r="F3"/>
       <c r="G3"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>125</v>
       </c>
@@ -2541,7 +2541,7 @@
       <c r="F4"/>
       <c r="G4"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>142</v>
       </c>
@@ -2556,7 +2556,7 @@
       <c r="F5"/>
       <c r="G5"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>53</v>
       </c>
@@ -2571,7 +2571,7 @@
       <c r="F6"/>
       <c r="G6"/>
     </row>
-    <row r="7" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7"/>
       <c r="B7"/>
       <c r="C7"/>
@@ -2580,7 +2580,7 @@
       <c r="F7"/>
       <c r="G7"/>
     </row>
-    <row r="8" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="23" t="s">
         <v>4</v>
       </c>
@@ -2612,7 +2612,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="50"/>
       <c r="B9" s="50"/>
       <c r="C9" s="50"/>
@@ -2620,7 +2620,7 @@
       <c r="F9" s="50"/>
       <c r="G9" s="50"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="50"/>
       <c r="B10" s="50"/>
       <c r="C10" s="50"/>
@@ -2628,7 +2628,7 @@
       <c r="F10" s="50"/>
       <c r="G10" s="50"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="50"/>
       <c r="B11" s="50"/>
       <c r="C11" s="50"/>
@@ -2636,7 +2636,7 @@
       <c r="F11" s="50"/>
       <c r="G11" s="50"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="50"/>
       <c r="B12" s="50"/>
       <c r="C12" s="50"/>
@@ -2644,7 +2644,7 @@
       <c r="F12" s="50"/>
       <c r="G12" s="50"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="50"/>
       <c r="B13" s="50"/>
       <c r="C13" s="50"/>
@@ -2690,17 +2690,17 @@
       <selection pane="bottomLeft" activeCell="L33" sqref="A10:L33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.265625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="18.86328125" style="7" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" style="7" customWidth="1"/>
     <col min="3" max="4" width="16" style="7" customWidth="1"/>
     <col min="5" max="5" width="18" style="6" customWidth="1"/>
-    <col min="6" max="6" width="16.1328125" style="6" customWidth="1"/>
-    <col min="7" max="7" width="34.3984375" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="34.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30.75" x14ac:dyDescent="0.9">
+    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>57</v>
       </c>
@@ -2710,7 +2710,7 @@
       <c r="E1"/>
       <c r="F1"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2"/>
       <c r="B2"/>
       <c r="C2"/>
@@ -2718,7 +2718,7 @@
       <c r="E2"/>
       <c r="F2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>123</v>
       </c>
@@ -2732,7 +2732,7 @@
       <c r="E3"/>
       <c r="F3"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>125</v>
       </c>
@@ -2746,7 +2746,7 @@
       <c r="E4"/>
       <c r="F4"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>142</v>
       </c>
@@ -2760,7 +2760,7 @@
       <c r="E5"/>
       <c r="F5"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>53</v>
       </c>
@@ -2774,7 +2774,7 @@
       <c r="E6"/>
       <c r="F6"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>54</v>
       </c>
@@ -2788,7 +2788,7 @@
       <c r="E7"/>
       <c r="F7"/>
     </row>
-    <row r="8" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8"/>
       <c r="B8"/>
       <c r="C8"/>
@@ -2796,7 +2796,7 @@
       <c r="E8"/>
       <c r="F8"/>
     </row>
-    <row r="9" spans="1:9" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
         <v>4</v>
       </c>
@@ -2825,31 +2825,31 @@
         <v>140</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="50"/>
       <c r="B10" s="50"/>
       <c r="C10" s="50"/>
       <c r="D10" s="50"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="50"/>
       <c r="B11" s="50"/>
       <c r="C11" s="50"/>
       <c r="D11" s="50"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="50"/>
       <c r="B12" s="50"/>
       <c r="C12" s="50"/>
       <c r="D12" s="50"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="50"/>
       <c r="B13" s="50"/>
       <c r="C13" s="50"/>
       <c r="D13" s="50"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="50"/>
       <c r="B14" s="50"/>
       <c r="C14" s="50"/>
@@ -2890,22 +2890,22 @@
       <selection pane="bottomLeft" activeCell="M35" sqref="A10:M35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.265625" customWidth="1"/>
-    <col min="2" max="2" width="18.86328125" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
     <col min="3" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="16.1328125" customWidth="1"/>
-    <col min="7" max="7" width="34.3984375" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" customWidth="1"/>
+    <col min="7" max="7" width="34.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30.75" x14ac:dyDescent="0.9">
+    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>123</v>
       </c>
@@ -2917,7 +2917,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>125</v>
       </c>
@@ -2929,7 +2929,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>142</v>
       </c>
@@ -2941,7 +2941,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>53</v>
       </c>
@@ -2953,7 +2953,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>54</v>
       </c>
@@ -2965,8 +2965,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="9" spans="1:9" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
         <v>4</v>
       </c>
@@ -3030,23 +3030,23 @@
       <selection pane="bottomLeft" activeCell="I33" sqref="A9:I33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.265625" customWidth="1"/>
-    <col min="2" max="2" width="18.86328125" customWidth="1"/>
-    <col min="3" max="3" width="17.86328125" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="7" width="18" customWidth="1"/>
-    <col min="8" max="8" width="16.1328125" customWidth="1"/>
-    <col min="9" max="9" width="34.3984375" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" customWidth="1"/>
+    <col min="9" max="9" width="34.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30.75" x14ac:dyDescent="0.9">
+    <row r="1" spans="1:11" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>123</v>
       </c>
@@ -3058,7 +3058,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>125</v>
       </c>
@@ -3070,7 +3070,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>142</v>
       </c>
@@ -3082,7 +3082,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>53</v>
       </c>
@@ -3094,8 +3094,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="8" spans="1:11" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="23" t="s">
         <v>4</v>
       </c>
@@ -3162,23 +3162,23 @@
       <selection pane="bottomLeft" activeCell="K29" sqref="A10:K29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.265625" customWidth="1"/>
-    <col min="2" max="2" width="18.86328125" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
     <col min="3" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="16.1328125" customWidth="1"/>
-    <col min="7" max="7" width="35.59765625" customWidth="1"/>
-    <col min="8" max="8" width="10.3984375" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" customWidth="1"/>
+    <col min="7" max="7" width="35.5703125" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30.75" x14ac:dyDescent="0.9">
+    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>123</v>
       </c>
@@ -3190,7 +3190,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>125</v>
       </c>
@@ -3202,7 +3202,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>142</v>
       </c>
@@ -3214,7 +3214,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>53</v>
       </c>
@@ -3226,7 +3226,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>66</v>
       </c>
@@ -3238,8 +3238,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="9" spans="1:9" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
         <v>4</v>
       </c>
@@ -3303,33 +3303,33 @@
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.1328125" customWidth="1"/>
-    <col min="2" max="2" width="43.1328125" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" customWidth="1"/>
+    <col min="2" max="2" width="43.140625" customWidth="1"/>
     <col min="3" max="16384" width="9" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="54" t="s">
+    <row r="1" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="54"/>
-    </row>
-    <row r="2" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B1" s="57"/>
+    </row>
+    <row r="2" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
     </row>
-    <row r="3" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
         <v>97</v>
       </c>
       <c r="B3" s="12"/>
     </row>
-    <row r="4" spans="1:2" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:2" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="14"/>
       <c r="B4" s="18"/>
     </row>
-    <row r="5" spans="1:2" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
         <v>48</v>
       </c>
@@ -3337,71 +3337,71 @@
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="19"/>
       <c r="B6" s="19"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="19"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="19"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="19"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="19"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="19"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="19"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="19"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="19"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="19"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="19"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="19"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="19"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="19"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="19"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="19"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="19"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="19"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="19"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="19"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="19"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="19"/>
     </row>
   </sheetData>
@@ -3436,24 +3436,24 @@
       <selection activeCell="I32" sqref="F19:I32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.265625" customWidth="1"/>
-    <col min="2" max="2" width="18.86328125" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
     <col min="3" max="4" width="16" customWidth="1"/>
     <col min="5" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="16.1328125" customWidth="1"/>
-    <col min="8" max="8" width="34.3984375" customWidth="1"/>
-    <col min="9" max="9" width="10.73046875" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" customWidth="1"/>
+    <col min="8" max="8" width="34.42578125" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" customWidth="1"/>
     <col min="10" max="10" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="30.75" x14ac:dyDescent="0.9">
+    <row r="1" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>123</v>
       </c>
@@ -3465,7 +3465,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>125</v>
       </c>
@@ -3477,7 +3477,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>142</v>
       </c>
@@ -3489,7 +3489,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>33</v>
       </c>
@@ -3501,7 +3501,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>32</v>
       </c>
@@ -3513,8 +3513,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="9" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
         <v>4</v>
       </c>
@@ -3580,15 +3580,15 @@
       <selection pane="bottomLeft" activeCell="H23" sqref="A10:H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="35.86328125" customWidth="1"/>
+    <col min="2" max="2" width="35.85546875" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="36.1328125" customWidth="1"/>
+    <col min="4" max="4" width="36.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30.75" x14ac:dyDescent="0.9">
+    <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="10" t="s">
         <v>74</v>
       </c>
@@ -3596,7 +3596,7 @@
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>123</v>
       </c>
@@ -3607,7 +3607,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>125</v>
       </c>
@@ -3618,7 +3618,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>82</v>
       </c>
@@ -3629,7 +3629,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>83</v>
       </c>
@@ -3640,7 +3640,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>156</v>
       </c>
@@ -3651,8 +3651,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="9" spans="1:6" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
         <v>77</v>
       </c>
@@ -3707,15 +3707,15 @@
       <selection pane="bottomLeft" activeCell="I37" sqref="A10:I37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="32.86328125" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="36.1328125" customWidth="1"/>
+    <col min="4" max="4" width="36.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30.75" x14ac:dyDescent="0.9">
+    <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="10" t="s">
         <v>74</v>
       </c>
@@ -3723,7 +3723,7 @@
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>123</v>
       </c>
@@ -3734,7 +3734,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>125</v>
       </c>
@@ -3745,7 +3745,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>82</v>
       </c>
@@ -3756,7 +3756,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>84</v>
       </c>
@@ -3767,7 +3767,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>156</v>
       </c>
@@ -3778,8 +3778,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="9" spans="1:6" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
         <v>77</v>
       </c>
@@ -3834,25 +3834,25 @@
       <selection pane="bottomLeft" activeCell="J35" sqref="A10:J35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="32.86328125" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="36.1328125" customWidth="1"/>
+    <col min="4" max="4" width="36.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30.75" x14ac:dyDescent="0.9">
-      <c r="A1" s="53" t="s">
+    <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="56" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>123</v>
       </c>
@@ -3863,7 +3863,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>125</v>
       </c>
@@ -3874,7 +3874,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>86</v>
       </c>
@@ -3885,7 +3885,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>88</v>
       </c>
@@ -3896,7 +3896,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>156</v>
       </c>
@@ -3907,8 +3907,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="9" spans="1:6" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
         <v>77</v>
       </c>
@@ -3966,15 +3966,15 @@
       <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="37.3984375" customWidth="1"/>
+    <col min="2" max="2" width="37.42578125" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="36.1328125" customWidth="1"/>
+    <col min="4" max="4" width="36.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30.75" x14ac:dyDescent="0.9">
+    <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="10" t="s">
         <v>74</v>
       </c>
@@ -3982,7 +3982,7 @@
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>123</v>
       </c>
@@ -3993,7 +3993,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>125</v>
       </c>
@@ -4004,7 +4004,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>82</v>
       </c>
@@ -4015,7 +4015,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>83</v>
       </c>
@@ -4026,7 +4026,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>156</v>
       </c>
@@ -4037,8 +4037,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="9" spans="1:6" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
         <v>77</v>
       </c>
@@ -4093,27 +4093,27 @@
       <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="35.73046875" customWidth="1"/>
+    <col min="2" max="2" width="35.7109375" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="15.59765625" customWidth="1"/>
-    <col min="5" max="5" width="33.86328125" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1"/>
+    <col min="5" max="5" width="33.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30.75" x14ac:dyDescent="0.9">
-      <c r="A1" s="53" t="s">
+    <row r="1" spans="1:7" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="56" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>123</v>
       </c>
@@ -4124,7 +4124,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>125</v>
       </c>
@@ -4135,7 +4135,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>82</v>
       </c>
@@ -4146,7 +4146,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>83</v>
       </c>
@@ -4157,7 +4157,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>156</v>
       </c>
@@ -4168,8 +4168,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="9" spans="1:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
         <v>4</v>
       </c>
@@ -4229,45 +4229,45 @@
       <selection activeCell="L35" sqref="A6:L35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.1328125" customWidth="1"/>
-    <col min="2" max="2" width="11.59765625" customWidth="1"/>
-    <col min="7" max="7" width="26.265625" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="7" max="7" width="26.28515625" customWidth="1"/>
     <col min="8" max="8" width="11" customWidth="1"/>
-    <col min="9" max="9" width="16.73046875" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30.75" x14ac:dyDescent="0.9">
-      <c r="A1" s="53" t="s">
+    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="56" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="58" t="s">
         <v>96</v>
       </c>
-      <c r="C3" s="56"/>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="56"/>
-      <c r="G3" s="56"/>
-      <c r="H3" s="56"/>
-      <c r="I3" s="57"/>
-    </row>
-    <row r="4" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="5" spans="1:9" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="59"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="60"/>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
         <v>77</v>
       </c>
@@ -4317,59 +4317,59 @@
       <selection activeCell="K30" sqref="A6:K30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.1328125" customWidth="1"/>
-    <col min="2" max="2" width="11.59765625" customWidth="1"/>
-    <col min="3" max="3" width="15.1328125" customWidth="1"/>
-    <col min="5" max="5" width="10.3984375" customWidth="1"/>
-    <col min="6" max="6" width="11.265625" customWidth="1"/>
-    <col min="7" max="7" width="12.1328125" customWidth="1"/>
-    <col min="8" max="9" width="15.73046875" customWidth="1"/>
-    <col min="10" max="10" width="18.1328125" customWidth="1"/>
-    <col min="11" max="11" width="26.265625" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" customWidth="1"/>
+    <col min="8" max="9" width="15.7109375" customWidth="1"/>
+    <col min="10" max="10" width="18.140625" customWidth="1"/>
+    <col min="11" max="11" width="26.28515625" customWidth="1"/>
     <col min="12" max="12" width="11" customWidth="1"/>
-    <col min="13" max="13" width="16.73046875" customWidth="1"/>
+    <col min="13" max="13" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="30.75" x14ac:dyDescent="0.9">
-      <c r="A1" s="53" t="s">
+    <row r="1" spans="1:13" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="56" t="s">
         <v>130</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="56"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="58" t="s">
         <v>96</v>
       </c>
-      <c r="C3" s="56"/>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="56"/>
-      <c r="G3" s="56"/>
-      <c r="H3" s="56"/>
-      <c r="I3" s="56"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="56"/>
-      <c r="L3" s="56"/>
-      <c r="M3" s="57"/>
-    </row>
-    <row r="4" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="5" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="59"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="59"/>
+      <c r="J3" s="59"/>
+      <c r="K3" s="59"/>
+      <c r="L3" s="59"/>
+      <c r="M3" s="60"/>
+    </row>
+    <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
         <v>77</v>
       </c>
@@ -4430,30 +4430,30 @@
       <selection activeCell="M34" sqref="A6:M34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.86328125" customWidth="1"/>
-    <col min="3" max="3" width="10.1328125" customWidth="1"/>
-    <col min="4" max="4" width="9.73046875" customWidth="1"/>
-    <col min="5" max="5" width="22.265625" customWidth="1"/>
-    <col min="6" max="6" width="11.3984375" customWidth="1"/>
-    <col min="7" max="7" width="15.3984375" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30.75" x14ac:dyDescent="0.9">
-      <c r="A1" s="53" t="s">
+    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="56" t="s">
         <v>99</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
       <c r="H1" s="10"/>
       <c r="I1" s="10"/>
     </row>
-    <row r="3" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>97</v>
       </c>
@@ -4464,8 +4464,8 @@
       <c r="F3" s="42"/>
       <c r="G3" s="43"/>
     </row>
-    <row r="4" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="5" spans="1:9" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
         <v>100</v>
       </c>
@@ -4503,34 +4503,34 @@
   </sheetPr>
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.73046875" customWidth="1"/>
-    <col min="2" max="2" width="37.3984375" customWidth="1"/>
+    <col min="1" max="1" width="28.7109375" customWidth="1"/>
+    <col min="2" max="2" width="37.42578125" customWidth="1"/>
     <col min="3" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="35.265625" customWidth="1"/>
-    <col min="7" max="7" width="15.73046875" customWidth="1"/>
-    <col min="8" max="8" width="12.3984375" customWidth="1"/>
-    <col min="9" max="16384" width="9.1328125" style="44"/>
+    <col min="5" max="5" width="35.28515625" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="44"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30.75" x14ac:dyDescent="0.9">
-      <c r="A1" s="53" t="s">
+    <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="56" t="s">
         <v>113</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>255</v>
       </c>
@@ -4542,7 +4542,7 @@
       </c>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>138</v>
       </c>
@@ -4552,15 +4552,15 @@
       </c>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="6" spans="1:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="B6" s="59" t="s">
+      <c r="B6" s="53" t="s">
         <v>252</v>
       </c>
-      <c r="C6" s="59" t="s">
+      <c r="C6" s="53" t="s">
         <v>253</v>
       </c>
       <c r="D6" s="52" t="s">
@@ -4579,7 +4579,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="51"/>
       <c r="B7" s="51"/>
       <c r="C7" s="51"/>
@@ -4589,7 +4589,7 @@
       <c r="G7" s="51"/>
       <c r="H7" s="51"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="51"/>
       <c r="B8" s="51"/>
       <c r="C8" s="51"/>
@@ -4599,7 +4599,7 @@
       <c r="G8" s="51"/>
       <c r="H8" s="51"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="51"/>
       <c r="B9" s="51"/>
       <c r="C9" s="51"/>
@@ -4609,7 +4609,7 @@
       <c r="G9" s="51"/>
       <c r="H9" s="51"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="51"/>
       <c r="B10" s="51"/>
       <c r="C10" s="51"/>
@@ -4619,7 +4619,7 @@
       <c r="G10" s="51"/>
       <c r="H10" s="51"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="51"/>
       <c r="B11" s="51"/>
       <c r="C11" s="51"/>
@@ -4654,406 +4654,406 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.1328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="8.3984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.73046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="8.3984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.73046875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.59765625" bestFit="1" customWidth="1"/>
-    <col min="13" max="17" width="8.3984375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.73046875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.3984375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.86328125" bestFit="1" customWidth="1"/>
-    <col min="21" max="31" width="8.3984375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="23.86328125" bestFit="1" customWidth="1"/>
-    <col min="33" max="37" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="17" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="31" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="37" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="14" bestFit="1" customWidth="1"/>
-    <col min="39" max="44" width="8.3984375" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="19.86328125" bestFit="1" customWidth="1"/>
-    <col min="46" max="58" width="8.3984375" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="6.59765625" bestFit="1" customWidth="1"/>
-    <col min="60" max="61" width="8.3984375" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="10.3984375" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="12.73046875" bestFit="1" customWidth="1"/>
+    <col min="39" max="44" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="46" max="58" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="60" max="61" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="64" max="64" width="7" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="8.3984375" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="25.86328125" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="7.73046875" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="6.3984375" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="6.1328125" bestFit="1" customWidth="1"/>
-    <col min="70" max="72" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="70" max="72" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="73" max="73" width="25" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="9.265625" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
         <v>193</v>
       </c>
@@ -5071,31 +5071,31 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection sqref="A1:F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.73046875" customWidth="1"/>
-    <col min="2" max="2" width="37.3984375" customWidth="1"/>
-    <col min="3" max="3" width="32.73046875" customWidth="1"/>
+    <col min="1" max="1" width="28.7109375" customWidth="1"/>
+    <col min="2" max="2" width="37.42578125" customWidth="1"/>
+    <col min="3" max="3" width="32.7109375" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="16.73046875" customWidth="1"/>
-    <col min="6" max="6" width="12.3984375" customWidth="1"/>
-    <col min="7" max="16384" width="9.1328125" style="44"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="44"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30.75" x14ac:dyDescent="0.9">
-      <c r="A1" s="53" t="s">
+    <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="56" t="s">
         <v>113</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>255</v>
       </c>
@@ -5107,7 +5107,7 @@
       </c>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>138</v>
       </c>
@@ -5117,12 +5117,12 @@
       </c>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="6" spans="1:6" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="B6" s="59" t="s">
+      <c r="B6" s="53" t="s">
         <v>257</v>
       </c>
       <c r="C6" s="24" t="s">
@@ -5138,7 +5138,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="51"/>
       <c r="B7" s="51"/>
       <c r="C7" s="51"/>
@@ -5146,7 +5146,7 @@
       <c r="E7" s="51"/>
       <c r="F7" s="51"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="51"/>
       <c r="B8" s="51"/>
       <c r="C8" s="51"/>
@@ -5154,7 +5154,7 @@
       <c r="E8" s="51"/>
       <c r="F8" s="51"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="51"/>
       <c r="B9" s="51"/>
       <c r="C9" s="51"/>
@@ -5162,7 +5162,7 @@
       <c r="E9" s="51"/>
       <c r="F9" s="51"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="51"/>
       <c r="B10" s="51"/>
       <c r="C10" s="51"/>
@@ -5170,7 +5170,7 @@
       <c r="E10" s="51"/>
       <c r="F10" s="51"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="51"/>
       <c r="B11" s="51"/>
       <c r="C11" s="51"/>
@@ -5199,31 +5199,31 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection sqref="A1:F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.73046875" customWidth="1"/>
-    <col min="2" max="2" width="37.3984375" customWidth="1"/>
-    <col min="3" max="3" width="32.73046875" customWidth="1"/>
+    <col min="1" max="1" width="28.7109375" customWidth="1"/>
+    <col min="2" max="2" width="37.42578125" customWidth="1"/>
+    <col min="3" max="3" width="32.7109375" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="16.73046875" customWidth="1"/>
-    <col min="6" max="6" width="12.3984375" customWidth="1"/>
-    <col min="7" max="16384" width="9.1328125" style="44"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="44"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30.75" x14ac:dyDescent="0.9">
-      <c r="A1" s="53" t="s">
+    <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="56" t="s">
         <v>113</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>255</v>
       </c>
@@ -5235,7 +5235,7 @@
       </c>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>138</v>
       </c>
@@ -5245,12 +5245,12 @@
       </c>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="6" spans="1:6" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="B6" s="59" t="s">
+      <c r="B6" s="53" t="s">
         <v>110</v>
       </c>
       <c r="C6" s="24" t="s">
@@ -5266,7 +5266,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="51"/>
       <c r="B7" s="51"/>
       <c r="C7" s="51"/>
@@ -5274,7 +5274,7 @@
       <c r="E7" s="51"/>
       <c r="F7" s="51"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="51"/>
       <c r="B8" s="51"/>
       <c r="C8" s="51"/>
@@ -5282,7 +5282,7 @@
       <c r="E8" s="51"/>
       <c r="F8" s="51"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="51"/>
       <c r="B9" s="51"/>
       <c r="C9" s="51"/>
@@ -5290,7 +5290,7 @@
       <c r="E9" s="51"/>
       <c r="F9" s="51"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="51"/>
       <c r="B10" s="51"/>
       <c r="C10" s="51"/>
@@ -5298,7 +5298,7 @@
       <c r="E10" s="51"/>
       <c r="F10" s="51"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="51"/>
       <c r="B11" s="51"/>
       <c r="C11" s="51"/>
@@ -5328,23 +5328,23 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomLeft" sqref="A1:H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="12.1328125" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="12.1328125" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="14.59765625" customWidth="1"/>
-    <col min="7" max="7" width="17.1328125" customWidth="1"/>
-    <col min="8" max="8" width="17.73046875" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" customWidth="1"/>
     <col min="9" max="9" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30.75" x14ac:dyDescent="0.9">
+    <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="10" t="s">
         <v>261</v>
       </c>
@@ -5352,20 +5352,20 @@
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="B3" s="58"/>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="58"/>
-    </row>
-    <row r="4" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="5" spans="1:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B3" s="61"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="61"/>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
         <v>111</v>
       </c>
@@ -5407,26 +5407,26 @@
   </sheetPr>
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomLeft" sqref="A1:I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="12.1328125" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="12.1328125" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="14.59765625" customWidth="1"/>
-    <col min="7" max="7" width="13.3984375" customWidth="1"/>
-    <col min="8" max="8" width="17.1328125" customWidth="1"/>
-    <col min="9" max="9" width="17.73046875" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" customWidth="1"/>
+    <col min="8" max="8" width="17.140625" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" customWidth="1"/>
     <col min="10" max="10" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30.75" x14ac:dyDescent="0.9">
+    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="10" t="s">
         <v>260</v>
       </c>
@@ -5434,21 +5434,21 @@
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="B3" s="58"/>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="58"/>
-      <c r="I3" s="58"/>
-    </row>
-    <row r="4" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="5" spans="1:9" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B3" s="61"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="61"/>
+      <c r="I3" s="61"/>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
         <v>111</v>
       </c>
@@ -5489,46 +5489,46 @@
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
-    <tabColor theme="3"/>
+    <tabColor rgb="FF00B0F0"/>
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.59765625" style="31" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" style="31" customWidth="1"/>
     <col min="2" max="2" width="52" style="31" customWidth="1"/>
-    <col min="3" max="16384" width="9.1328125" style="31"/>
+    <col min="3" max="16384" width="9.140625" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="30" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A1" s="53" t="s">
+    <row r="1" spans="1:2" s="30" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="56" t="s">
         <v>262</v>
       </c>
-      <c r="B1" s="53"/>
-    </row>
-    <row r="2" spans="1:2" s="30" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B1" s="56"/>
+    </row>
+    <row r="2" spans="1:2" s="30" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
       <c r="B2"/>
     </row>
-    <row r="3" spans="1:2" s="30" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" s="30" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
         <v>97</v>
       </c>
       <c r="B3" s="38"/>
     </row>
-    <row r="4" spans="1:2" s="30" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:2" s="30" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="14"/>
       <c r="B4" s="18"/>
     </row>
-    <row r="5" spans="1:2" ht="338.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="60" t="s">
+    <row r="5" spans="1:2" ht="338.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="54" t="s">
         <v>263</v>
       </c>
-      <c r="B5" s="61"/>
+      <c r="B5" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5551,30 +5551,30 @@
       <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.73046875" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="16.1328125" customWidth="1"/>
-    <col min="5" max="5" width="36.1328125" customWidth="1"/>
-    <col min="6" max="6" width="9.73046875" customWidth="1"/>
-    <col min="7" max="7" width="10.3984375" customWidth="1"/>
-    <col min="8" max="16384" width="9.1328125" style="40"/>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="5" max="5" width="36.140625" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="40"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30.75" x14ac:dyDescent="0.9">
-      <c r="A1" s="53" t="s">
+    <row r="1" spans="1:7" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
@@ -5583,7 +5583,7 @@
       <c r="F2" s="15"/>
       <c r="G2" s="16"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>123</v>
       </c>
@@ -5598,7 +5598,7 @@
       <c r="F3" s="15"/>
       <c r="G3" s="16"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>125</v>
       </c>
@@ -5613,7 +5613,7 @@
       <c r="F4" s="15"/>
       <c r="G4" s="16"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
@@ -5628,7 +5628,7 @@
       <c r="F5" s="15"/>
       <c r="G5" s="16"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
@@ -5643,7 +5643,7 @@
       <c r="F6" s="15"/>
       <c r="G6" s="16"/>
     </row>
-    <row r="7" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="20"/>
       <c r="B7" s="20"/>
       <c r="C7" s="20"/>
@@ -5652,7 +5652,7 @@
       <c r="F7" s="20"/>
       <c r="G7" s="21"/>
     </row>
-    <row r="8" spans="1:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="23" t="s">
         <v>4</v>
       </c>
@@ -5709,32 +5709,32 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.86328125" customWidth="1"/>
-    <col min="2" max="2" width="22.86328125" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="16.1328125" customWidth="1"/>
-    <col min="6" max="6" width="34.3984375" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" customWidth="1"/>
+    <col min="6" max="6" width="34.42578125" customWidth="1"/>
     <col min="7" max="7" width="9"/>
-    <col min="8" max="8" width="10.1328125" customWidth="1"/>
-    <col min="9" max="16384" width="9.1328125" style="39"/>
+    <col min="8" max="8" width="10.140625" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="39"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30.75" x14ac:dyDescent="0.9">
-      <c r="A1" s="53" t="s">
+    <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>123</v>
       </c>
@@ -5746,7 +5746,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>125</v>
       </c>
@@ -5758,7 +5758,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>127</v>
       </c>
@@ -5770,7 +5770,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>86</v>
       </c>
@@ -5782,7 +5782,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>3</v>
       </c>
@@ -5794,10 +5794,10 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="3"/>
     </row>
-    <row r="9" spans="1:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
         <v>4</v>
       </c>
@@ -5860,34 +5860,34 @@
       <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.73046875" customWidth="1"/>
-    <col min="2" max="2" width="20.265625" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="16.1328125" customWidth="1"/>
-    <col min="6" max="6" width="14.3984375" customWidth="1"/>
-    <col min="7" max="7" width="31.3984375" customWidth="1"/>
-    <col min="8" max="8" width="11.1328125" customWidth="1"/>
-    <col min="9" max="9" width="11.265625" customWidth="1"/>
-    <col min="10" max="16384" width="9.1328125" style="25"/>
+    <col min="5" max="5" width="16.140625" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
+    <col min="7" max="7" width="31.42578125" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30.75" x14ac:dyDescent="0.9">
-      <c r="A1" s="53" t="s">
+    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>123</v>
       </c>
@@ -5898,7 +5898,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>125</v>
       </c>
@@ -5909,7 +5909,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>23</v>
       </c>
@@ -5920,7 +5920,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
@@ -5931,8 +5931,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="8" spans="1:9" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="23" t="s">
         <v>4</v>
       </c>
@@ -5996,34 +5996,34 @@
       <selection pane="bottomLeft" activeCell="G32" sqref="A9:G32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.265625" customWidth="1"/>
-    <col min="2" max="2" width="18.86328125" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="16.1328125" customWidth="1"/>
-    <col min="6" max="6" width="11.1328125" customWidth="1"/>
-    <col min="7" max="7" width="34.3984375" customWidth="1"/>
-    <col min="8" max="8" width="10.73046875" customWidth="1"/>
-    <col min="9" max="9" width="15.1328125" customWidth="1"/>
-    <col min="10" max="16384" width="9.1328125" style="27"/>
+    <col min="5" max="5" width="16.140625" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" customWidth="1"/>
+    <col min="7" max="7" width="34.42578125" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30.75" x14ac:dyDescent="0.9">
-      <c r="A1" s="53" t="s">
+    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>123</v>
       </c>
@@ -6035,7 +6035,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>125</v>
       </c>
@@ -6047,7 +6047,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>23</v>
       </c>
@@ -6059,7 +6059,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
@@ -6071,8 +6071,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="8" spans="1:9" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="23" t="s">
         <v>4</v>
       </c>
@@ -6136,34 +6136,34 @@
       <selection pane="bottomLeft" activeCell="H27" sqref="A11:H27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.265625" customWidth="1"/>
-    <col min="2" max="2" width="18.86328125" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="7" width="16.1328125" customWidth="1"/>
-    <col min="8" max="8" width="11.86328125" customWidth="1"/>
-    <col min="9" max="9" width="34.3984375" customWidth="1"/>
-    <col min="11" max="11" width="9.73046875" customWidth="1"/>
+    <col min="5" max="7" width="16.140625" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" customWidth="1"/>
+    <col min="9" max="9" width="34.42578125" customWidth="1"/>
+    <col min="11" max="11" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30.75" x14ac:dyDescent="0.9">
-      <c r="A1" s="53" t="s">
+    <row r="1" spans="1:11" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>123</v>
       </c>
@@ -6175,7 +6175,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>125</v>
       </c>
@@ -6187,7 +6187,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>23</v>
       </c>
@@ -6199,7 +6199,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
@@ -6211,7 +6211,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>21</v>
       </c>
@@ -6223,7 +6223,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>22</v>
       </c>
@@ -6235,10 +6235,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="3"/>
     </row>
-    <row r="10" spans="1:11" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="23" t="s">
         <v>4</v>
       </c>
@@ -6314,24 +6314,24 @@
       <selection pane="bottomLeft" activeCell="H33" sqref="A10:H33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.265625" customWidth="1"/>
-    <col min="2" max="2" width="18.86328125" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
     <col min="3" max="4" width="16" customWidth="1"/>
     <col min="5" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="16.1328125" customWidth="1"/>
-    <col min="8" max="8" width="34.3984375" customWidth="1"/>
-    <col min="9" max="9" width="10.73046875" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" customWidth="1"/>
+    <col min="8" max="8" width="34.42578125" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" customWidth="1"/>
     <col min="10" max="10" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="30.75" x14ac:dyDescent="0.9">
+    <row r="1" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>123</v>
       </c>
@@ -6343,7 +6343,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>125</v>
       </c>
@@ -6355,7 +6355,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>142</v>
       </c>
@@ -6367,7 +6367,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>33</v>
       </c>
@@ -6379,7 +6379,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>32</v>
       </c>
@@ -6391,8 +6391,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="9" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
         <v>4</v>
       </c>
@@ -6424,19 +6424,19 @@
         <v>140</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F10" s="8"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F11" s="8"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F12" s="8"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F13" s="8"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F14" s="8"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All changes made made during the process of updating the data as of 6-8-2018
</commit_message>
<xml_diff>
--- a/Atomistic-Class1/WebFF-Class1-DataTemplate.xlsx
+++ b/Atomistic-Class1/WebFF-Class1-DataTemplate.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="18195" windowHeight="8190" firstSheet="28" activeTab="32"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="18195" windowHeight="8190" firstSheet="16" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="20" r:id="rId1"/>
@@ -3432,8 +3432,8 @@
   </sheetPr>
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I32" sqref="F19:I32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3555,7 +3555,7 @@
       <formula1>"? , kcal, kJ"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4">
-      <formula1>"?, Kd*[1+cos(N*Phi-Phi0)], Kd*[1+cos(N*Phi+Phi0)], .5*Kd*[1+cos(N*Phi-Phi0)], .5*Kd*[1+cos(N*Phi+Phi0)]"</formula1>
+      <formula1>"?, Kd*[1+cos(N*Phi-Phi0)], Kd*[1+cos(N*Phi+Phi0)], 0.5*Kd*[1+cos(N*Phi-Phi0)], 0.5*Kd*[1+cos(N*Phi+Phi0)]"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
       <formula1>"CHARMM"</formula1>
@@ -5407,7 +5407,7 @@
   </sheetPr>
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" sqref="A1:I5"/>
     </sheetView>

</xml_diff>